<commit_message>
Some Cleric and Gnome feats
</commit_message>
<xml_diff>
--- a/activities.xlsx
+++ b/activities.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/eb76e5660c890129/Personal/Projects/Design/PECS/work assets/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="1666" documentId="13_ncr:40009_{E3EB266C-7612-416D-8781-7A2BED99FA57}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{A81FD29F-6D4B-4147-BB70-F7DDA5126A5F}"/>
+  <xr:revisionPtr revIDLastSave="1941" documentId="13_ncr:40009_{E3EB266C-7612-416D-8781-7A2BED99FA57}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{0AA81A4A-6D70-4B7A-BFC5-4E02C4FF7956}"/>
   <bookViews>
-    <workbookView xWindow="21570" yWindow="0" windowWidth="33570" windowHeight="20970" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="4290" yWindow="630" windowWidth="33570" windowHeight="20970" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Work" sheetId="2" r:id="rId1"/>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6084" uniqueCount="1227">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6244" uniqueCount="1293">
   <si>
     <t>name</t>
   </si>
@@ -3836,6 +3836,207 @@
   <si>
     <t>You bring a weapon into metaphysical concordance with your deity's beliefs. This action has the trait corresponding to the chosen alignment component.
 When you use this action, you touch a weapon. For 1 round, that weapon deals an additional 1d6 damage of the chosen type to creatures of the opposed alignment. For example, if you chose good, the weapon would deal an extra 1d6 good damage to evil creatures. If you Align an Armament again, any previously aligned armament loses its additional damage.</t>
+  </si>
+  <si>
+    <t>Heroic Recovery</t>
+  </si>
+  <si>
+    <t>Using this action grants the effect to your ally independently of the heal spell. Cast a heal spell afterwards to properly expend the spell slot.</t>
+  </si>
+  <si>
+    <t>The restorative power of your healing invigorates the recipient. If the next action you use is to cast heal targeting a single living creature and the target regains Hit Points from the spell, it also gains three bonuses until the end of its next turn: a +5-foot status bonus to its Speed, a +1 status bonus to attack rolls, and a +1 status bonus to damage rolls.</t>
+  </si>
+  <si>
+    <t>Heroic Recovery (Originator)</t>
+  </si>
+  <si>
+    <t>Replenishment of War</t>
+  </si>
+  <si>
+    <t>Favored Weapon</t>
+  </si>
+  <si>
+    <t>Striking out against your enemies draws praise and protection from your deity. When you damage a creature with a Strike using your deity's favored weapon, you gain a number of temporary Hit Points equal to half your level, or equal to your level if the Strike was a critical hit. These temporary Hit Points last until the start of your next turn.</t>
+  </si>
+  <si>
+    <t>Defensive Recovery</t>
+  </si>
+  <si>
+    <t>Your faith provides temporary protection in addition to healing. If the next action you use is to cast harm or heal on a single target and the target regains Hit Points from the spell, it also gains a +2 status bonus to AC and saving throws for 1 round.</t>
+  </si>
+  <si>
+    <t>Defensive Recovery (Originator)</t>
+  </si>
+  <si>
+    <t>Replenishment of War (Originator)</t>
+  </si>
+  <si>
+    <t>Has_Feat(Creature.type, 'Shared Replenishment') ? 1 : 0</t>
+  </si>
+  <si>
+    <t>!Has_Feat(Creature.type, 'Shared Replenishment') ? 1 : 0</t>
+  </si>
+  <si>
+    <t>You have a banishment spell prepared.</t>
+  </si>
+  <si>
+    <t>You critically hit a creature that is not on its home plane.</t>
+  </si>
+  <si>
+    <t>The force of your blow sends your victim back to its home plane. You expend a banishment spell you have prepared, affecting the creature you critically hit without needing to cast the spell. The creature can attempt to resist the spell as normal.</t>
+  </si>
+  <si>
+    <t>Swift Banishment</t>
+  </si>
+  <si>
+    <t>Banishment (Caster)</t>
+  </si>
+  <si>
+    <t>Dismiss Eternal Bane</t>
+  </si>
+  <si>
+    <t>Eternal Bane Dismissed</t>
+  </si>
+  <si>
+    <t>Until you have the Shared Replenishment feat, activating Replenishment of War will only affect yourself regardless of the selected target.</t>
+  </si>
+  <si>
+    <t>Dismiss Eternal Blessing</t>
+  </si>
+  <si>
+    <t>Eternal Blessing</t>
+  </si>
+  <si>
+    <t>Bless</t>
+  </si>
+  <si>
+    <t>You're continuously surrounded by a bless spell. You can use this activity to grant the effect of the spell to your allies when they enter its radius.</t>
+  </si>
+  <si>
+    <t>You're continuously surrounded by a bane spell. You can use this activity to Dismiss the spell; it will return automatically after 1 minute.</t>
+  </si>
+  <si>
+    <t>You're continuously surrounded by a bless spell. You can use this activity to Dismiss the spell; it will return automatically after 1 minute.</t>
+  </si>
+  <si>
+    <t>Resurrectionist</t>
+  </si>
+  <si>
+    <t>You can cause a creature you bring back from the brink of death to thrive and continue healing. After restoring Hit Points to a dying creature or bringing a dead creature back to life and restoring Hit Points to it, you grant that creature fast healing 5 for 1 minute. This fast healing ends if the creature is knocked unconscious.</t>
+  </si>
+  <si>
+    <t>Resurrectionist (Originator)</t>
+  </si>
+  <si>
+    <t>Echoing Channel</t>
+  </si>
+  <si>
+    <t>When you pull forth positive or negative energy, you also create a smaller pocket of that energy. If the next action you use is to cast a 2-action harm or heal to heal or damage a single creature, choose one additional creature adjacent to either you or the target. Target that creature with a 1-action version of the same spell. This spell is the same level as the 2-action harm or heal you cast and doesn’t cost another spell slot.</t>
+  </si>
+  <si>
+    <t>In play, you can choose one additional creature to apply the effect. There is no change to the spell you cast.</t>
+  </si>
+  <si>
+    <t>three times a day</t>
+  </si>
+  <si>
+    <t>Dance of Intercesion</t>
+  </si>
+  <si>
+    <t>You either performed in or stood witness to the dance used to invoke the Celestial Dragon and can harness a sliver of their power. You Stride in a dance up to half your Speed, attempting a DC 35 Performance check. You can perform this dance up to three times per day. The second time you do so in the same day, use the degree of success one worse than your actual roll on the Performance check. The third time in a day, use the degree of success two lower than your actual roll.</t>
+  </si>
+  <si>
+    <t>You perform the movements of the Dance of Intercession so gracefully that you evoke a glimmer of the memory of the Celestial Dragon's awesome power. You cast the 3-action version of either 9th-level harm or heal at any point during your Stride. This does not use any spell slots.</t>
+  </si>
+  <si>
+    <t>As critical success, but the spell is 7th level instead of 9th as you stumble through the movements.</t>
+  </si>
+  <si>
+    <t>As critical success, but the spell is 5th level instead of 9th as you stumble through the movements.</t>
+  </si>
+  <si>
+    <t>You fail to remember the steps of the dance. You gain no additional effect beyond Striding half your Speed, and you can't attempt the Dance of Intercession again until your next daily preparations.</t>
+  </si>
+  <si>
+    <t>Heal</t>
+  </si>
+  <si>
+    <t>showSpells/1/level</t>
+  </si>
+  <si>
+    <t>showSpells/1/name</t>
+  </si>
+  <si>
+    <t>showSpells/2/level</t>
+  </si>
+  <si>
+    <t>showSpells/2/name</t>
+  </si>
+  <si>
+    <t>showSpells/3/level</t>
+  </si>
+  <si>
+    <t>showSpells/3/name</t>
+  </si>
+  <si>
+    <t>Harm</t>
+  </si>
+  <si>
+    <t>showSpells/4/level</t>
+  </si>
+  <si>
+    <t>showSpells/4/name</t>
+  </si>
+  <si>
+    <t>showSpells/5/level</t>
+  </si>
+  <si>
+    <t>showSpells/5/name</t>
+  </si>
+  <si>
+    <t>You have a heal spell prepared and you aren't flat-footed to the source of the damage.</t>
+  </si>
+  <si>
+    <t>Any ally within 30 feet that you can heal with your heal spell would take damage from an attack or effect from a source you can observe.</t>
+  </si>
+  <si>
+    <t>You can manipulate the same energies that the aeon orbs use to sustain life. You cast heal on the triggering target. Instead of its normal effects, the heal spell reduces the triggering damage by an amount equal to the Hit Points a 1-action heal spell of that level would have recovered. As usual, if this reduces the damage to 0, it might also remove additional effects of the triggering attack, such as injury poisons.</t>
+  </si>
+  <si>
+    <t>Cast a prepared heal spell as indicated.</t>
+  </si>
+  <si>
+    <t>You can expend a banishment spell for swift banishment in your spell list. Alternatively, you can just cast the spell to the same effect and treat it as though it took no actions and had no traits.
+If you have Improved Swift Banishment, you can expend any prepared spell of 5th level or higher in your spell list.</t>
+  </si>
+  <si>
+    <t>Metamagic Channel</t>
+  </si>
+  <si>
+    <t>Deep understanding of divine revelations into the nature of vital essence allows you to freely manipulate the effects of your positive or negative energy. Use 1 metamagic action that you can perform that normally takes 1 action and can be applied to the harm or heal spell. If you use it in this way, its effects apply only to a harm or heal spell.</t>
+  </si>
+  <si>
+    <t>Inventive Offensive</t>
+  </si>
+  <si>
+    <t>Vibrant Display</t>
+  </si>
+  <si>
+    <t>You can jury-rig your weapons to perform in unexpected ways. When you use this ability, add one of the following weapon traits to a melee weapon you wield: deadly d6, disarm, nonlethal, shove, trip, versatile B, versatile P, or versatile S. You cannot add a trait that the weapon already has. The weapon retains this trait until you a successfully hit and deal damage with the weapon. The weapon retains this trait only while you wield it, and you can have only one weapon modified in this way at any time.
+If you have expert proficiency in Crafting, you can use this feat as a 2-action activity. If you have legendary proficiency in Crafting, you can apply two weapon traits from the list when using this feat.</t>
+  </si>
+  <si>
+    <t>Gnome</t>
+  </si>
+  <si>
+    <t>Once every 10 minutes, when you use the Feint action, you can compare your Deception check result to the Perception DCs of all adjacent creatures rather than just one creature within melee reach. It's possible to get a different degree of success for each target.
+These changes are imprecise and usually short-lived, so while they allow you to periodically change your appearance in unpredictable ways, they are of little use in providing camouflage or aiding a disguise.</t>
+  </si>
+  <si>
+    <t>once every 10 minutes</t>
+  </si>
+  <si>
+    <t>To apply an additional weapon trait if you have legendary proficiency in Crafting, use this ability a second time.</t>
   </si>
 </sst>
 </file>
@@ -4319,7 +4520,7 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="10" borderId="0" xfId="19" applyAlignment="1"/>
@@ -4333,6 +4534,9 @@
     <xf numFmtId="0" fontId="1" fillId="15" borderId="0" xfId="24"/>
     <xf numFmtId="0" fontId="1" fillId="14" borderId="0" xfId="23"/>
     <xf numFmtId="0" fontId="1" fillId="15" borderId="0" xfId="24" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -4378,7 +4582,27 @@
     <cellStyle name="Total" xfId="17" builtinId="25" customBuiltin="1"/>
     <cellStyle name="Warning Text" xfId="14" builtinId="11" customBuiltin="1"/>
   </cellStyles>
-  <dxfs count="45">
+  <dxfs count="59">
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <font>
         <color rgb="FF9C0006"/>
@@ -4576,6 +4800,13 @@
       </fill>
     </dxf>
     <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
       <font>
         <color rgb="FF9C0006"/>
       </font>
@@ -4626,9 +4857,122 @@
       </fill>
     </dxf>
     <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
       <fill>
         <patternFill>
-          <bgColor rgb="FFFF0000"/>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
         </patternFill>
       </fill>
     </dxf>
@@ -5091,23 +5435,23 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:LZ145"/>
+  <dimension ref="A1:MN155"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="LW14" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="ML2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="LZ47" sqref="LZ47"/>
+      <selection pane="bottomRight" activeCell="MN4" sqref="MN4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="37.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="338" width="27.42578125" style="1" customWidth="1"/>
-    <col min="339" max="16384" width="9.140625" style="1"/>
+    <col min="2" max="352" width="27.42578125" style="1" customWidth="1"/>
+    <col min="353" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:338" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:352" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -6122,8 +6466,50 @@
       <c r="LZ1" t="s">
         <v>1224</v>
       </c>
+      <c r="MA1" t="s">
+        <v>1227</v>
+      </c>
+      <c r="MB1" t="s">
+        <v>1231</v>
+      </c>
+      <c r="MC1" t="s">
+        <v>1234</v>
+      </c>
+      <c r="MD1" t="s">
+        <v>1243</v>
+      </c>
+      <c r="ME1" t="s">
+        <v>1245</v>
+      </c>
+      <c r="MF1" t="s">
+        <v>1249</v>
+      </c>
+      <c r="MG1" t="s">
+        <v>1248</v>
+      </c>
+      <c r="MH1" t="s">
+        <v>1254</v>
+      </c>
+      <c r="MI1" t="s">
+        <v>1257</v>
+      </c>
+      <c r="MJ1" t="s">
+        <v>1261</v>
+      </c>
+      <c r="MK1" t="s">
+        <v>1261</v>
+      </c>
+      <c r="ML1" t="s">
+        <v>1284</v>
+      </c>
+      <c r="MM1" t="s">
+        <v>1286</v>
+      </c>
+      <c r="MN1" t="s">
+        <v>1287</v>
+      </c>
     </row>
-    <row r="2" spans="1:338" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:352" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>1</v>
       </c>
@@ -7126,8 +7512,38 @@
       <c r="LZ2" s="1" t="s">
         <v>51</v>
       </c>
+      <c r="MA2" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="MC2" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="MD2" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="ME2" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="MG2" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="MI2" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="MJ2" s="1" t="s">
+        <v>198</v>
+      </c>
+      <c r="MK2" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="ML2" s="1" t="s">
+        <v>127</v>
+      </c>
+      <c r="MM2" s="1" t="s">
+        <v>198</v>
+      </c>
     </row>
-    <row r="3" spans="1:338" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:352" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>20</v>
       </c>
@@ -7326,8 +7742,29 @@
       <c r="LX3" s="1" t="s">
         <v>1223</v>
       </c>
+      <c r="MA3" s="1" t="s">
+        <v>1228</v>
+      </c>
+      <c r="MB3" s="1" t="s">
+        <v>1247</v>
+      </c>
+      <c r="MC3" s="1" t="s">
+        <v>1223</v>
+      </c>
+      <c r="MD3" s="1" t="s">
+        <v>1283</v>
+      </c>
+      <c r="MI3" s="1" t="s">
+        <v>1259</v>
+      </c>
+      <c r="MK3" s="1" t="s">
+        <v>1282</v>
+      </c>
+      <c r="MM3" s="1" t="s">
+        <v>1292</v>
+      </c>
     </row>
-    <row r="4" spans="1:338" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:352" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
         <v>3</v>
       </c>
@@ -8294,8 +8731,41 @@
       <c r="LZ4" s="2" t="s">
         <v>321</v>
       </c>
+      <c r="MA4" s="2" t="s">
+        <v>321</v>
+      </c>
+      <c r="MB4" s="2" t="s">
+        <v>321</v>
+      </c>
+      <c r="MC4" s="2" t="s">
+        <v>321</v>
+      </c>
+      <c r="MD4" s="2" t="s">
+        <v>321</v>
+      </c>
+      <c r="ME4" s="2" t="s">
+        <v>144</v>
+      </c>
+      <c r="MG4" s="2" t="s">
+        <v>144</v>
+      </c>
+      <c r="MI4" s="2" t="s">
+        <v>321</v>
+      </c>
+      <c r="MJ4" s="2" t="s">
+        <v>188</v>
+      </c>
+      <c r="MK4" s="2" t="s">
+        <v>188</v>
+      </c>
+      <c r="ML4" s="2" t="s">
+        <v>321</v>
+      </c>
+      <c r="MM4" s="2" t="s">
+        <v>1289</v>
+      </c>
     </row>
-    <row r="5" spans="1:338" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:352" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
         <v>4</v>
       </c>
@@ -8974,8 +9444,26 @@
       <c r="LZ5" s="2" t="s">
         <v>213</v>
       </c>
+      <c r="MA5" s="2" t="s">
+        <v>144</v>
+      </c>
+      <c r="MC5" s="2" t="s">
+        <v>144</v>
+      </c>
+      <c r="MI5" s="2" t="s">
+        <v>144</v>
+      </c>
+      <c r="MJ5" s="2" t="s">
+        <v>321</v>
+      </c>
+      <c r="MK5" s="2" t="s">
+        <v>321</v>
+      </c>
+      <c r="ML5" s="2" t="s">
+        <v>144</v>
+      </c>
     </row>
-    <row r="6" spans="1:338" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:352" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
         <v>11</v>
       </c>
@@ -9333,8 +9821,17 @@
       <c r="LZ6" s="2" t="s">
         <v>146</v>
       </c>
+      <c r="MA6" s="2" t="s">
+        <v>316</v>
+      </c>
+      <c r="MC6" s="2" t="s">
+        <v>316</v>
+      </c>
+      <c r="MI6" s="2" t="s">
+        <v>316</v>
+      </c>
     </row>
-    <row r="7" spans="1:338" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:352" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
         <v>12</v>
       </c>
@@ -9573,7 +10070,7 @@
         <v>316</v>
       </c>
     </row>
-    <row r="8" spans="1:338" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:352" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
         <v>13</v>
       </c>
@@ -9719,7 +10216,7 @@
         <v>181</v>
       </c>
     </row>
-    <row r="9" spans="1:338" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:352" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
         <v>34</v>
       </c>
@@ -9745,7 +10242,7 @@
         <v>289</v>
       </c>
     </row>
-    <row r="10" spans="1:338" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:352" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
         <v>37</v>
       </c>
@@ -9759,7 +10256,7 @@
         <v>897</v>
       </c>
     </row>
-    <row r="11" spans="1:338" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:352" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
         <v>6</v>
       </c>
@@ -10057,8 +10554,14 @@
       <c r="LO11" s="1" t="s">
         <v>976</v>
       </c>
+      <c r="MD11" s="1" t="s">
+        <v>1240</v>
+      </c>
+      <c r="MK11" s="1" t="s">
+        <v>1279</v>
+      </c>
     </row>
-    <row r="12" spans="1:338" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:352" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
         <v>10</v>
       </c>
@@ -10284,8 +10787,14 @@
       <c r="LY12" s="1" t="s">
         <v>1218</v>
       </c>
+      <c r="MD12" s="1" t="s">
+        <v>1241</v>
+      </c>
+      <c r="MK12" s="1" t="s">
+        <v>1280</v>
+      </c>
     </row>
-    <row r="13" spans="1:338" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:352" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
         <v>5</v>
       </c>
@@ -10440,12 +10949,12 @@
         <v>1</v>
       </c>
     </row>
-    <row r="14" spans="1:338" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:352" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
         <v>937</v>
       </c>
     </row>
-    <row r="15" spans="1:338" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:352" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
         <v>48</v>
       </c>
@@ -10455,8 +10964,11 @@
       <c r="JM15" s="1">
         <v>1</v>
       </c>
+      <c r="MJ15" s="1">
+        <v>3</v>
+      </c>
     </row>
-    <row r="16" spans="1:338" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:352" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
         <v>35</v>
       </c>
@@ -10467,7 +10979,7 @@
         <v>1207</v>
       </c>
     </row>
-    <row r="17" spans="1:338" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:352" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
         <v>18</v>
       </c>
@@ -10583,8 +11095,14 @@
       <c r="LZ17" s="1" t="s">
         <v>123</v>
       </c>
+      <c r="MJ17" s="1" t="s">
+        <v>1260</v>
+      </c>
+      <c r="MN17" s="1" t="s">
+        <v>1291</v>
+      </c>
     </row>
-    <row r="18" spans="1:338" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:352" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
         <v>19</v>
       </c>
@@ -10711,8 +11229,14 @@
       <c r="LZ18" s="1">
         <v>5</v>
       </c>
+      <c r="MJ18" s="1">
+        <v>144000</v>
+      </c>
+      <c r="MN18" s="1">
+        <v>1000</v>
+      </c>
     </row>
-    <row r="19" spans="1:338" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:352" x14ac:dyDescent="0.25">
       <c r="A19" s="1" t="s">
         <v>36</v>
       </c>
@@ -10723,7 +11247,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="20" spans="1:338" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:352" x14ac:dyDescent="0.25">
       <c r="A20" s="1" t="s">
         <v>21</v>
       </c>
@@ -10773,7 +11297,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="21" spans="1:338" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:352" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>1019</v>
       </c>
@@ -10786,8 +11310,14 @@
       <c r="LW21" s="1" t="b">
         <v>1</v>
       </c>
+      <c r="MA21" s="1" t="b">
+        <v>1</v>
+      </c>
+      <c r="MB21" s="1" t="b">
+        <v>1</v>
+      </c>
     </row>
-    <row r="22" spans="1:338" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:352" x14ac:dyDescent="0.25">
       <c r="A22" s="1" t="s">
         <v>1017</v>
       </c>
@@ -11802,8 +12332,50 @@
       <c r="LZ22" s="1" t="s">
         <v>1002</v>
       </c>
+      <c r="MA22" s="1" t="s">
+        <v>1002</v>
+      </c>
+      <c r="MB22" s="1" t="s">
+        <v>1002</v>
+      </c>
+      <c r="MC22" s="1" t="s">
+        <v>1002</v>
+      </c>
+      <c r="MD22" s="1" t="s">
+        <v>999</v>
+      </c>
+      <c r="ME22" s="1" t="s">
+        <v>1000</v>
+      </c>
+      <c r="MF22" s="1" t="s">
+        <v>1002</v>
+      </c>
+      <c r="MG22" s="1" t="s">
+        <v>1000</v>
+      </c>
+      <c r="MH22" s="1" t="s">
+        <v>1002</v>
+      </c>
+      <c r="MI22" s="1" t="s">
+        <v>1000</v>
+      </c>
+      <c r="MJ22" s="1" t="s">
+        <v>1000</v>
+      </c>
+      <c r="MK22" s="1" t="s">
+        <v>1000</v>
+      </c>
+      <c r="ML22" s="1" t="s">
+        <v>1000</v>
+      </c>
+      <c r="MM22" s="1" t="s">
+        <v>1000</v>
+      </c>
+      <c r="MN22" s="1" t="s">
+        <v>1000</v>
+      </c>
     </row>
-    <row r="23" spans="1:338" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:352" x14ac:dyDescent="0.25">
       <c r="A23" s="1" t="s">
         <v>1033</v>
       </c>
@@ -11835,7 +12407,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="24" spans="1:338" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:352" x14ac:dyDescent="0.25">
       <c r="A24" s="1" t="s">
         <v>1189</v>
       </c>
@@ -11926,8 +12498,11 @@
       <c r="IZ24" s="1" t="s">
         <v>1195</v>
       </c>
+      <c r="MB24" s="1" t="s">
+        <v>1232</v>
+      </c>
     </row>
-    <row r="25" spans="1:338" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:352" x14ac:dyDescent="0.25">
       <c r="A25" s="1" t="s">
         <v>2</v>
       </c>
@@ -12942,8 +13517,50 @@
       <c r="LZ25" s="1" t="s">
         <v>1226</v>
       </c>
+      <c r="MA25" s="1" t="s">
+        <v>1229</v>
+      </c>
+      <c r="MB25" s="1" t="s">
+        <v>1233</v>
+      </c>
+      <c r="MC25" s="1" t="s">
+        <v>1235</v>
+      </c>
+      <c r="MD25" s="1" t="s">
+        <v>1242</v>
+      </c>
+      <c r="ME25" s="1" t="s">
+        <v>1252</v>
+      </c>
+      <c r="MF25" s="1" t="s">
+        <v>1251</v>
+      </c>
+      <c r="MG25" s="1" t="s">
+        <v>1253</v>
+      </c>
+      <c r="MH25" s="1" t="s">
+        <v>1255</v>
+      </c>
+      <c r="MI25" s="1" t="s">
+        <v>1258</v>
+      </c>
+      <c r="MJ25" s="1" t="s">
+        <v>1262</v>
+      </c>
+      <c r="MK25" s="1" t="s">
+        <v>1281</v>
+      </c>
+      <c r="ML25" s="1" t="s">
+        <v>1285</v>
+      </c>
+      <c r="MM25" s="1" t="s">
+        <v>1288</v>
+      </c>
+      <c r="MN25" s="13" t="s">
+        <v>1290</v>
+      </c>
     </row>
-    <row r="26" spans="1:338" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:352" x14ac:dyDescent="0.25">
       <c r="A26" s="1" t="s">
         <v>38</v>
       </c>
@@ -12960,7 +13577,7 @@
         <v>701</v>
       </c>
     </row>
-    <row r="27" spans="1:338" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:352" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A27" s="3" t="s">
         <v>14</v>
       </c>
@@ -13006,8 +13623,14 @@
       <c r="IS27" s="3" t="s">
         <v>764</v>
       </c>
+      <c r="MJ27" s="3" t="s">
+        <v>1263</v>
+      </c>
+      <c r="MK27" s="3" t="s">
+        <v>1263</v>
+      </c>
     </row>
-    <row r="28" spans="1:338" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:352" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A28" s="3" t="s">
         <v>15</v>
       </c>
@@ -13062,8 +13685,14 @@
       <c r="IS28" s="3" t="s">
         <v>765</v>
       </c>
+      <c r="MJ28" s="3" t="s">
+        <v>1264</v>
+      </c>
+      <c r="MK28" s="3" t="s">
+        <v>1264</v>
+      </c>
     </row>
-    <row r="29" spans="1:338" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:352" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A29" s="3" t="s">
         <v>16</v>
       </c>
@@ -13124,8 +13753,14 @@
       <c r="HT29" s="3" t="s">
         <v>684</v>
       </c>
+      <c r="MJ29" s="3" t="s">
+        <v>1265</v>
+      </c>
+      <c r="MK29" s="3" t="s">
+        <v>1265</v>
+      </c>
     </row>
-    <row r="30" spans="1:338" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:352" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A30" s="3" t="s">
         <v>17</v>
       </c>
@@ -13171,8 +13806,14 @@
       <c r="IS30" s="3" t="s">
         <v>766</v>
       </c>
+      <c r="MJ30" s="3" t="s">
+        <v>1266</v>
+      </c>
+      <c r="MK30" s="3" t="s">
+        <v>1266</v>
+      </c>
     </row>
-    <row r="31" spans="1:338" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:352" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A31" s="9" t="s">
         <v>1007</v>
       </c>
@@ -13185,8 +13826,11 @@
       <c r="IQ31" s="9">
         <v>2</v>
       </c>
+      <c r="MF31" s="9">
+        <v>-1</v>
+      </c>
     </row>
-    <row r="32" spans="1:338" s="7" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:352" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A32" s="7" t="s">
         <v>25</v>
       </c>
@@ -13196,8 +13840,11 @@
       <c r="AZ32" s="7" t="s">
         <v>232</v>
       </c>
+      <c r="MB32" s="7" t="s">
+        <v>1239</v>
+      </c>
     </row>
-    <row r="33" spans="1:338" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:351" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A33" s="4" t="s">
         <v>22</v>
       </c>
@@ -13208,12 +13855,12 @@
         <v>2</v>
       </c>
     </row>
-    <row r="34" spans="1:338" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:351" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A34" s="4" t="s">
         <v>926</v>
       </c>
     </row>
-    <row r="35" spans="1:338" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:351" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A35" s="4" t="s">
         <v>998</v>
       </c>
@@ -13221,12 +13868,12 @@
         <v>996</v>
       </c>
     </row>
-    <row r="36" spans="1:338" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:351" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A36" s="4" t="s">
         <v>938</v>
       </c>
     </row>
-    <row r="37" spans="1:338" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:351" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A37" s="4" t="s">
         <v>7</v>
       </c>
@@ -13554,8 +14201,35 @@
       <c r="LZ37" s="4">
         <v>10</v>
       </c>
+      <c r="MA37" s="4">
+        <v>10</v>
+      </c>
+      <c r="MB37" s="4">
+        <v>15</v>
+      </c>
+      <c r="MC37" s="4">
+        <v>10</v>
+      </c>
+      <c r="MD37" s="4">
+        <v>0</v>
+      </c>
+      <c r="ME37" s="4">
+        <v>100</v>
+      </c>
+      <c r="MF37" s="4">
+        <v>-1</v>
+      </c>
+      <c r="MG37" s="4">
+        <v>100</v>
+      </c>
+      <c r="MH37" s="4">
+        <v>100</v>
+      </c>
+      <c r="MM37" s="4">
+        <v>-1</v>
+      </c>
     </row>
-    <row r="38" spans="1:338" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:351" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A38" s="4" t="s">
         <v>997</v>
       </c>
@@ -13563,7 +14237,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="39" spans="1:338" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:351" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A39" s="4" t="s">
         <v>8</v>
       </c>
@@ -13915,8 +14589,35 @@
       <c r="LZ39" s="4" t="s">
         <v>1225</v>
       </c>
+      <c r="MA39" s="4" t="s">
+        <v>1230</v>
+      </c>
+      <c r="MB39" s="4" t="s">
+        <v>1231</v>
+      </c>
+      <c r="MC39" s="4" t="s">
+        <v>1236</v>
+      </c>
+      <c r="MD39" s="4" t="s">
+        <v>1244</v>
+      </c>
+      <c r="ME39" s="4" t="s">
+        <v>1246</v>
+      </c>
+      <c r="MF39" s="4" t="s">
+        <v>1250</v>
+      </c>
+      <c r="MG39" s="4" t="s">
+        <v>1246</v>
+      </c>
+      <c r="MH39" s="4" t="s">
+        <v>1256</v>
+      </c>
+      <c r="MM39" s="4" t="s">
+        <v>1286</v>
+      </c>
     </row>
-    <row r="40" spans="1:338" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:351" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A40" s="4" t="s">
         <v>9</v>
       </c>
@@ -14265,8 +14966,35 @@
       <c r="LZ40" s="4" t="s">
         <v>1224</v>
       </c>
+      <c r="MA40" s="4" t="s">
+        <v>1227</v>
+      </c>
+      <c r="MB40" s="4" t="s">
+        <v>1231</v>
+      </c>
+      <c r="MC40" s="4" t="s">
+        <v>1234</v>
+      </c>
+      <c r="MD40" s="4" t="s">
+        <v>1243</v>
+      </c>
+      <c r="ME40" s="4" t="s">
+        <v>1245</v>
+      </c>
+      <c r="MF40" s="4" t="s">
+        <v>1249</v>
+      </c>
+      <c r="MG40" s="4" t="s">
+        <v>1245</v>
+      </c>
+      <c r="MH40" s="4" t="s">
+        <v>1254</v>
+      </c>
+      <c r="MM40" s="4" t="s">
+        <v>1286</v>
+      </c>
     </row>
-    <row r="41" spans="1:338" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:351" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A41" s="4" t="s">
         <v>1015</v>
       </c>
@@ -14348,8 +15076,23 @@
       <c r="LZ41" s="4" t="s">
         <v>1016</v>
       </c>
+      <c r="MA41" s="4" t="s">
+        <v>1016</v>
+      </c>
+      <c r="MB41" s="4" t="s">
+        <v>1016</v>
+      </c>
+      <c r="MC41" s="4" t="s">
+        <v>1016</v>
+      </c>
+      <c r="MD41" s="4" t="s">
+        <v>1016</v>
+      </c>
+      <c r="MH41" s="4" t="s">
+        <v>1016</v>
+      </c>
     </row>
-    <row r="42" spans="1:338" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:351" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A42" s="4" t="s">
         <v>994</v>
       </c>
@@ -14357,30 +15100,33 @@
         <v>1</v>
       </c>
     </row>
-    <row r="43" spans="1:338" s="7" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:351" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A43" s="7" t="s">
         <v>29</v>
       </c>
       <c r="AQ43" s="7" t="s">
         <v>191</v>
       </c>
+      <c r="MB43" s="7" t="s">
+        <v>1238</v>
+      </c>
     </row>
-    <row r="44" spans="1:338" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:351" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A44" s="4" t="s">
         <v>927</v>
       </c>
     </row>
-    <row r="45" spans="1:338" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:351" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A45" s="4" t="s">
         <v>940</v>
       </c>
     </row>
-    <row r="46" spans="1:338" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:351" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A46" s="4" t="s">
         <v>1022</v>
       </c>
     </row>
-    <row r="47" spans="1:338" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:351" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A47" s="4" t="s">
         <v>1023</v>
       </c>
@@ -14399,8 +15145,11 @@
       <c r="LZ47" s="4" t="s">
         <v>1225</v>
       </c>
+      <c r="MC47" s="4" t="s">
+        <v>1236</v>
+      </c>
     </row>
-    <row r="48" spans="1:338" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:351" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A48" s="4" t="s">
         <v>26</v>
       </c>
@@ -14428,8 +15177,20 @@
       <c r="LZ48" s="4">
         <v>10</v>
       </c>
+      <c r="MA48" s="4">
+        <v>10</v>
+      </c>
+      <c r="MB48" s="4">
+        <v>15</v>
+      </c>
+      <c r="MC48" s="4">
+        <v>10</v>
+      </c>
+      <c r="MH48" s="4">
+        <v>100</v>
+      </c>
     </row>
-    <row r="49" spans="1:338" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:346" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A49" s="4" t="s">
         <v>27</v>
       </c>
@@ -14475,8 +15236,20 @@
       <c r="LZ49" s="4" t="s">
         <v>1224</v>
       </c>
+      <c r="MA49" s="4" t="s">
+        <v>1227</v>
+      </c>
+      <c r="MB49" s="4" t="s">
+        <v>1237</v>
+      </c>
+      <c r="MC49" s="4" t="s">
+        <v>1234</v>
+      </c>
+      <c r="MH49" s="4" t="s">
+        <v>1254</v>
+      </c>
     </row>
-    <row r="50" spans="1:338" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:346" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A50" s="4" t="s">
         <v>28</v>
       </c>
@@ -14522,8 +15295,20 @@
       <c r="LZ50" s="4" t="s">
         <v>1224</v>
       </c>
+      <c r="MA50" s="4" t="s">
+        <v>1227</v>
+      </c>
+      <c r="MB50" s="4" t="s">
+        <v>1231</v>
+      </c>
+      <c r="MC50" s="4" t="s">
+        <v>1234</v>
+      </c>
+      <c r="MH50" s="4" t="s">
+        <v>1254</v>
+      </c>
     </row>
-    <row r="51" spans="1:338" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:346" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A51" s="4" t="s">
         <v>1021</v>
       </c>
@@ -14557,8 +15342,26 @@
       <c r="KG51" s="4" t="s">
         <v>1017</v>
       </c>
+      <c r="LW51" s="4" t="s">
+        <v>1017</v>
+      </c>
+      <c r="LZ51" s="4" t="s">
+        <v>1017</v>
+      </c>
+      <c r="MA51" s="4" t="s">
+        <v>1017</v>
+      </c>
+      <c r="MB51" s="4" t="s">
+        <v>1016</v>
+      </c>
+      <c r="MC51" s="4" t="s">
+        <v>1017</v>
+      </c>
+      <c r="MH51" s="4" t="s">
+        <v>1017</v>
+      </c>
     </row>
-    <row r="52" spans="1:338" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:346" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A52" s="4" t="s">
         <v>47</v>
       </c>
@@ -14566,7 +15369,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="53" spans="1:338" s="7" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:346" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A53" s="7" t="s">
         <v>33</v>
       </c>
@@ -14576,26 +15379,32 @@
       <c r="KG53" s="7" t="s">
         <v>935</v>
       </c>
+      <c r="MB53" s="7" t="s">
+        <v>1238</v>
+      </c>
     </row>
-    <row r="54" spans="1:338" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:346" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A54" s="4" t="s">
         <v>928</v>
       </c>
     </row>
-    <row r="55" spans="1:338" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:346" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A55" s="4" t="s">
         <v>939</v>
       </c>
     </row>
-    <row r="56" spans="1:338" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:346" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A56" s="4" t="s">
         <v>30</v>
       </c>
       <c r="AQ56" s="4">
         <v>500</v>
       </c>
+      <c r="MB56" s="4">
+        <v>15</v>
+      </c>
     </row>
-    <row r="57" spans="1:338" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:346" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A57" s="4" t="s">
         <v>31</v>
       </c>
@@ -14605,8 +15414,11 @@
       <c r="KG57" s="4" t="s">
         <v>936</v>
       </c>
+      <c r="MB57" s="4" t="s">
+        <v>1231</v>
+      </c>
     </row>
-    <row r="58" spans="1:338" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:346" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A58" s="4" t="s">
         <v>32</v>
       </c>
@@ -14616,16 +15428,22 @@
       <c r="KG58" s="4" t="s">
         <v>852</v>
       </c>
+      <c r="MB58" s="4" t="s">
+        <v>1231</v>
+      </c>
     </row>
-    <row r="59" spans="1:338" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:346" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A59" s="4" t="s">
         <v>1020</v>
       </c>
       <c r="KG59" s="4" t="s">
         <v>1016</v>
       </c>
+      <c r="MB59" s="4" t="s">
+        <v>1017</v>
+      </c>
     </row>
-    <row r="60" spans="1:338" s="5" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:346" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A60" s="5" t="s">
         <v>23</v>
       </c>
@@ -14654,7 +15472,7 @@
         <v>263</v>
       </c>
     </row>
-    <row r="61" spans="1:338" s="5" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:346" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A61" s="5" t="s">
         <v>24</v>
       </c>
@@ -14683,7 +15501,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="62" spans="1:338" s="8" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:346" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A62" s="8" t="s">
         <v>41</v>
       </c>
@@ -14700,7 +15518,7 @@
         <v>631</v>
       </c>
     </row>
-    <row r="63" spans="1:338" s="6" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:346" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A63" s="6" t="s">
         <v>40</v>
       </c>
@@ -14717,7 +15535,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="64" spans="1:338" s="6" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:346" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A64" s="6" t="s">
         <v>39</v>
       </c>
@@ -14734,7 +15552,7 @@
         <v>953</v>
       </c>
     </row>
-    <row r="65" spans="1:324" s="8" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:349" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A65" s="8" t="s">
         <v>44</v>
       </c>
@@ -14742,7 +15560,7 @@
         <v>631</v>
       </c>
     </row>
-    <row r="66" spans="1:324" s="6" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:349" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A66" s="6" t="s">
         <v>43</v>
       </c>
@@ -14750,7 +15568,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="67" spans="1:324" s="6" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:349" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A67" s="6" t="s">
         <v>42</v>
       </c>
@@ -14758,7 +15576,7 @@
         <v>630</v>
       </c>
     </row>
-    <row r="68" spans="1:324" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:349" x14ac:dyDescent="0.25">
       <c r="A68" s="1" t="s">
         <v>49</v>
       </c>
@@ -14766,7 +15584,7 @@
         <v>816</v>
       </c>
     </row>
-    <row r="69" spans="1:324" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:349" x14ac:dyDescent="0.25">
       <c r="A69" s="1" t="s">
         <v>46</v>
       </c>
@@ -14785,8 +15603,14 @@
       <c r="LL69" s="1">
         <v>10</v>
       </c>
+      <c r="MJ69" s="1">
+        <v>9</v>
+      </c>
+      <c r="MK69" s="1">
+        <v>9</v>
+      </c>
     </row>
-    <row r="70" spans="1:324" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:349" x14ac:dyDescent="0.25">
       <c r="A70" s="1" t="s">
         <v>45</v>
       </c>
@@ -14805,130 +15629,148 @@
       <c r="LL70" s="1" t="s">
         <v>968</v>
       </c>
+      <c r="MJ70" s="1" t="s">
+        <v>1274</v>
+      </c>
+      <c r="MK70" s="1" t="s">
+        <v>1274</v>
+      </c>
     </row>
-    <row r="71" spans="1:324" s="12" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A71" s="10" t="s">
-        <v>1046</v>
-      </c>
-      <c r="AO71" s="12">
-        <v>1</v>
-      </c>
-      <c r="KB71" s="12">
-        <v>6</v>
+    <row r="71" spans="1:349" x14ac:dyDescent="0.25">
+      <c r="A71" s="1" t="s">
+        <v>1268</v>
+      </c>
+      <c r="MJ71" s="1">
+        <v>9</v>
+      </c>
+      <c r="MK71" s="1">
+        <v>9</v>
       </c>
     </row>
-    <row r="72" spans="1:324" s="9" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A72" s="11" t="s">
-        <v>1047</v>
-      </c>
-      <c r="AO72" s="9" t="s">
-        <v>1096</v>
-      </c>
-      <c r="KB72" s="9" t="s">
-        <v>1102</v>
+    <row r="72" spans="1:349" x14ac:dyDescent="0.25">
+      <c r="A72" s="1" t="s">
+        <v>1269</v>
+      </c>
+      <c r="MJ72" s="1" t="s">
+        <v>1267</v>
+      </c>
+      <c r="MK72" s="1" t="s">
+        <v>1267</v>
       </c>
     </row>
-    <row r="73" spans="1:324" s="9" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A73" s="11" t="s">
-        <v>1048</v>
-      </c>
-      <c r="AO73" s="9" t="s">
-        <v>1097</v>
-      </c>
-      <c r="KB73" s="9" t="s">
-        <v>1097</v>
+    <row r="73" spans="1:349" x14ac:dyDescent="0.25">
+      <c r="A73" s="1" t="s">
+        <v>1270</v>
+      </c>
+      <c r="MJ73" s="1">
+        <v>7</v>
+      </c>
+      <c r="MK73" s="1">
+        <v>7</v>
       </c>
     </row>
-    <row r="74" spans="1:324" s="9" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A74" s="11" t="s">
-        <v>1049</v>
-      </c>
-      <c r="KB74" s="9" t="s">
-        <v>1099</v>
+    <row r="74" spans="1:349" x14ac:dyDescent="0.25">
+      <c r="A74" s="1" t="s">
+        <v>1271</v>
+      </c>
+      <c r="MJ74" s="1" t="s">
+        <v>1274</v>
+      </c>
+      <c r="MK74" s="1" t="s">
+        <v>1274</v>
       </c>
     </row>
-    <row r="75" spans="1:324" s="9" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A75" s="11" t="s">
-        <v>1050</v>
-      </c>
-      <c r="KB75" s="9" t="s">
-        <v>1167</v>
+    <row r="75" spans="1:349" x14ac:dyDescent="0.25">
+      <c r="A75" s="1" t="s">
+        <v>1272</v>
+      </c>
+      <c r="MJ75" s="1">
+        <v>7</v>
+      </c>
+      <c r="MK75" s="1">
+        <v>7</v>
       </c>
     </row>
-    <row r="76" spans="1:324" s="12" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A76" s="10" t="s">
-        <v>1051</v>
-      </c>
-      <c r="AO76" s="12">
-        <v>3</v>
-      </c>
-      <c r="KB76" s="12">
-        <v>7</v>
+    <row r="76" spans="1:349" x14ac:dyDescent="0.25">
+      <c r="A76" s="1" t="s">
+        <v>1273</v>
+      </c>
+      <c r="MJ76" s="1" t="s">
+        <v>1267</v>
+      </c>
+      <c r="MK76" s="1" t="s">
+        <v>1267</v>
       </c>
     </row>
-    <row r="77" spans="1:324" s="9" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A77" s="11" t="s">
-        <v>1052</v>
-      </c>
-      <c r="AO77" s="9" t="s">
-        <v>1098</v>
-      </c>
-      <c r="KB77" s="9" t="s">
-        <v>1103</v>
+    <row r="77" spans="1:349" x14ac:dyDescent="0.25">
+      <c r="A77" s="1" t="s">
+        <v>1275</v>
+      </c>
+      <c r="MJ77" s="1">
+        <v>5</v>
+      </c>
+      <c r="MK77" s="1">
+        <v>5</v>
       </c>
     </row>
-    <row r="78" spans="1:324" s="9" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A78" s="11" t="s">
-        <v>1053</v>
-      </c>
-      <c r="AO78" s="9" t="s">
-        <v>1097</v>
-      </c>
-      <c r="KB78" s="9" t="s">
-        <v>1097</v>
+    <row r="78" spans="1:349" x14ac:dyDescent="0.25">
+      <c r="A78" s="1" t="s">
+        <v>1276</v>
+      </c>
+      <c r="MJ78" s="1" t="s">
+        <v>1274</v>
+      </c>
+      <c r="MK78" s="1" t="s">
+        <v>1274</v>
       </c>
     </row>
-    <row r="79" spans="1:324" s="9" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A79" s="11" t="s">
-        <v>1054</v>
-      </c>
-      <c r="KB79" s="9" t="s">
-        <v>1099</v>
+    <row r="79" spans="1:349" x14ac:dyDescent="0.25">
+      <c r="A79" s="1" t="s">
+        <v>1277</v>
+      </c>
+      <c r="MJ79" s="1">
+        <v>5</v>
+      </c>
+      <c r="MK79" s="1">
+        <v>5</v>
       </c>
     </row>
-    <row r="80" spans="1:324" s="9" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A80" s="11" t="s">
-        <v>1055</v>
-      </c>
-      <c r="KB80" s="9" t="s">
-        <v>1167</v>
+    <row r="80" spans="1:349" x14ac:dyDescent="0.25">
+      <c r="A80" s="1" t="s">
+        <v>1278</v>
+      </c>
+      <c r="MJ80" s="1" t="s">
+        <v>1267</v>
+      </c>
+      <c r="MK80" s="1" t="s">
+        <v>1267</v>
       </c>
     </row>
     <row r="81" spans="1:288" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A81" s="10" t="s">
-        <v>1056</v>
+        <v>1046</v>
       </c>
       <c r="AO81" s="12">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="KB81" s="12">
-        <v>8</v>
+        <v>6</v>
       </c>
     </row>
     <row r="82" spans="1:288" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A82" s="11" t="s">
-        <v>1057</v>
+        <v>1047</v>
       </c>
       <c r="AO82" s="9" t="s">
-        <v>1099</v>
+        <v>1096</v>
       </c>
       <c r="KB82" s="9" t="s">
-        <v>1104</v>
+        <v>1102</v>
       </c>
     </row>
     <row r="83" spans="1:288" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A83" s="11" t="s">
-        <v>1058</v>
+        <v>1048</v>
       </c>
       <c r="AO83" s="9" t="s">
         <v>1097</v>
@@ -14939,15 +15781,15 @@
     </row>
     <row r="84" spans="1:288" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A84" s="11" t="s">
-        <v>1059</v>
+        <v>1049</v>
       </c>
       <c r="KB84" s="9" t="s">
-        <v>1100</v>
+        <v>1099</v>
       </c>
     </row>
     <row r="85" spans="1:288" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A85" s="11" t="s">
-        <v>1060</v>
+        <v>1050</v>
       </c>
       <c r="KB85" s="9" t="s">
         <v>1167</v>
@@ -14955,29 +15797,29 @@
     </row>
     <row r="86" spans="1:288" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A86" s="10" t="s">
-        <v>1061</v>
+        <v>1051</v>
       </c>
       <c r="AO86" s="12">
+        <v>3</v>
+      </c>
+      <c r="KB86" s="12">
         <v>7</v>
-      </c>
-      <c r="KB86" s="12">
-        <v>9</v>
       </c>
     </row>
     <row r="87" spans="1:288" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A87" s="11" t="s">
-        <v>1062</v>
+        <v>1052</v>
       </c>
       <c r="AO87" s="9" t="s">
-        <v>1100</v>
+        <v>1098</v>
       </c>
       <c r="KB87" s="9" t="s">
-        <v>1105</v>
+        <v>1103</v>
       </c>
     </row>
     <row r="88" spans="1:288" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A88" s="11" t="s">
-        <v>1063</v>
+        <v>1053</v>
       </c>
       <c r="AO88" s="9" t="s">
         <v>1097</v>
@@ -14988,15 +15830,15 @@
     </row>
     <row r="89" spans="1:288" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A89" s="11" t="s">
-        <v>1064</v>
+        <v>1054</v>
       </c>
       <c r="KB89" s="9" t="s">
-        <v>1100</v>
+        <v>1099</v>
       </c>
     </row>
     <row r="90" spans="1:288" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A90" s="11" t="s">
-        <v>1065</v>
+        <v>1055</v>
       </c>
       <c r="KB90" s="9" t="s">
         <v>1167</v>
@@ -15004,29 +15846,29 @@
     </row>
     <row r="91" spans="1:288" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A91" s="10" t="s">
-        <v>1066</v>
+        <v>1056</v>
       </c>
       <c r="AO91" s="12">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="KB91" s="12">
-        <v>10</v>
+        <v>8</v>
       </c>
     </row>
     <row r="92" spans="1:288" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A92" s="11" t="s">
-        <v>1067</v>
+        <v>1057</v>
       </c>
       <c r="AO92" s="9" t="s">
-        <v>1101</v>
+        <v>1099</v>
       </c>
       <c r="KB92" s="9" t="s">
-        <v>1106</v>
+        <v>1104</v>
       </c>
     </row>
     <row r="93" spans="1:288" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A93" s="11" t="s">
-        <v>1068</v>
+        <v>1058</v>
       </c>
       <c r="AO93" s="9" t="s">
         <v>1097</v>
@@ -15037,15 +15879,15 @@
     </row>
     <row r="94" spans="1:288" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A94" s="11" t="s">
-        <v>1069</v>
+        <v>1059</v>
       </c>
       <c r="KB94" s="9" t="s">
-        <v>1101</v>
+        <v>1100</v>
       </c>
     </row>
     <row r="95" spans="1:288" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A95" s="11" t="s">
-        <v>1070</v>
+        <v>1060</v>
       </c>
       <c r="KB95" s="9" t="s">
         <v>1167</v>
@@ -15053,29 +15895,29 @@
     </row>
     <row r="96" spans="1:288" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A96" s="10" t="s">
-        <v>1071</v>
+        <v>1061</v>
       </c>
       <c r="AO96" s="12">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="KB96" s="12">
-        <v>11</v>
+        <v>9</v>
       </c>
     </row>
     <row r="97" spans="1:288" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A97" s="11" t="s">
-        <v>1072</v>
+        <v>1062</v>
       </c>
       <c r="AO97" s="9" t="s">
-        <v>1102</v>
+        <v>1100</v>
       </c>
       <c r="KB97" s="9" t="s">
-        <v>1168</v>
+        <v>1105</v>
       </c>
     </row>
     <row r="98" spans="1:288" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A98" s="11" t="s">
-        <v>1073</v>
+        <v>1063</v>
       </c>
       <c r="AO98" s="9" t="s">
         <v>1097</v>
@@ -15086,15 +15928,15 @@
     </row>
     <row r="99" spans="1:288" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A99" s="11" t="s">
-        <v>1074</v>
+        <v>1064</v>
       </c>
       <c r="KB99" s="9" t="s">
-        <v>1101</v>
+        <v>1100</v>
       </c>
     </row>
     <row r="100" spans="1:288" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A100" s="11" t="s">
-        <v>1075</v>
+        <v>1065</v>
       </c>
       <c r="KB100" s="9" t="s">
         <v>1167</v>
@@ -15102,29 +15944,29 @@
     </row>
     <row r="101" spans="1:288" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A101" s="10" t="s">
-        <v>1076</v>
+        <v>1066</v>
       </c>
       <c r="AO101" s="12">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="KB101" s="12">
-        <v>12</v>
+        <v>10</v>
       </c>
     </row>
     <row r="102" spans="1:288" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A102" s="11" t="s">
-        <v>1077</v>
+        <v>1067</v>
       </c>
       <c r="AO102" s="9" t="s">
-        <v>1103</v>
+        <v>1101</v>
       </c>
       <c r="KB102" s="9" t="s">
-        <v>1169</v>
+        <v>1106</v>
       </c>
     </row>
     <row r="103" spans="1:288" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A103" s="11" t="s">
-        <v>1078</v>
+        <v>1068</v>
       </c>
       <c r="AO103" s="9" t="s">
         <v>1097</v>
@@ -15135,15 +15977,15 @@
     </row>
     <row r="104" spans="1:288" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A104" s="11" t="s">
-        <v>1079</v>
+        <v>1069</v>
       </c>
       <c r="KB104" s="9" t="s">
-        <v>1102</v>
+        <v>1101</v>
       </c>
     </row>
     <row r="105" spans="1:288" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A105" s="11" t="s">
-        <v>1080</v>
+        <v>1070</v>
       </c>
       <c r="KB105" s="9" t="s">
         <v>1167</v>
@@ -15151,29 +15993,29 @@
     </row>
     <row r="106" spans="1:288" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A106" s="10" t="s">
-        <v>1081</v>
+        <v>1071</v>
       </c>
       <c r="AO106" s="12">
-        <v>15</v>
+        <v>11</v>
       </c>
       <c r="KB106" s="12">
-        <v>13</v>
+        <v>11</v>
       </c>
     </row>
     <row r="107" spans="1:288" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A107" s="11" t="s">
-        <v>1082</v>
+        <v>1072</v>
       </c>
       <c r="AO107" s="9" t="s">
-        <v>1104</v>
+        <v>1102</v>
       </c>
       <c r="KB107" s="9" t="s">
-        <v>1170</v>
+        <v>1168</v>
       </c>
     </row>
     <row r="108" spans="1:288" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A108" s="11" t="s">
-        <v>1083</v>
+        <v>1073</v>
       </c>
       <c r="AO108" s="9" t="s">
         <v>1097</v>
@@ -15184,15 +16026,15 @@
     </row>
     <row r="109" spans="1:288" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A109" s="11" t="s">
-        <v>1084</v>
+        <v>1074</v>
       </c>
       <c r="KB109" s="9" t="s">
-        <v>1102</v>
+        <v>1101</v>
       </c>
     </row>
     <row r="110" spans="1:288" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A110" s="11" t="s">
-        <v>1085</v>
+        <v>1075</v>
       </c>
       <c r="KB110" s="9" t="s">
         <v>1167</v>
@@ -15200,29 +16042,29 @@
     </row>
     <row r="111" spans="1:288" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A111" s="10" t="s">
-        <v>1086</v>
+        <v>1076</v>
       </c>
       <c r="AO111" s="12">
-        <v>17</v>
+        <v>13</v>
       </c>
       <c r="KB111" s="12">
-        <v>14</v>
+        <v>12</v>
       </c>
     </row>
     <row r="112" spans="1:288" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A112" s="11" t="s">
-        <v>1087</v>
+        <v>1077</v>
       </c>
       <c r="AO112" s="9" t="s">
-        <v>1105</v>
+        <v>1103</v>
       </c>
       <c r="KB112" s="9" t="s">
-        <v>1171</v>
+        <v>1169</v>
       </c>
     </row>
     <row r="113" spans="1:288" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A113" s="11" t="s">
-        <v>1088</v>
+        <v>1078</v>
       </c>
       <c r="AO113" s="9" t="s">
         <v>1097</v>
@@ -15233,15 +16075,15 @@
     </row>
     <row r="114" spans="1:288" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A114" s="11" t="s">
-        <v>1089</v>
+        <v>1079</v>
       </c>
       <c r="KB114" s="9" t="s">
-        <v>1103</v>
+        <v>1102</v>
       </c>
     </row>
     <row r="115" spans="1:288" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A115" s="11" t="s">
-        <v>1090</v>
+        <v>1080</v>
       </c>
       <c r="KB115" s="9" t="s">
         <v>1167</v>
@@ -15249,29 +16091,29 @@
     </row>
     <row r="116" spans="1:288" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A116" s="10" t="s">
-        <v>1091</v>
+        <v>1081</v>
       </c>
       <c r="AO116" s="12">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="KB116" s="12">
-        <v>15</v>
+        <v>13</v>
       </c>
     </row>
     <row r="117" spans="1:288" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A117" s="11" t="s">
-        <v>1092</v>
+        <v>1082</v>
       </c>
       <c r="AO117" s="9" t="s">
-        <v>1106</v>
+        <v>1104</v>
       </c>
       <c r="KB117" s="9" t="s">
-        <v>1172</v>
+        <v>1170</v>
       </c>
     </row>
     <row r="118" spans="1:288" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A118" s="11" t="s">
-        <v>1093</v>
+        <v>1083</v>
       </c>
       <c r="AO118" s="9" t="s">
         <v>1097</v>
@@ -15282,15 +16124,15 @@
     </row>
     <row r="119" spans="1:288" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A119" s="11" t="s">
-        <v>1094</v>
+        <v>1084</v>
       </c>
       <c r="KB119" s="9" t="s">
-        <v>1103</v>
+        <v>1102</v>
       </c>
     </row>
     <row r="120" spans="1:288" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A120" s="11" t="s">
-        <v>1095</v>
+        <v>1085</v>
       </c>
       <c r="KB120" s="9" t="s">
         <v>1167</v>
@@ -15298,23 +16140,32 @@
     </row>
     <row r="121" spans="1:288" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A121" s="10" t="s">
-        <v>1141</v>
+        <v>1086</v>
+      </c>
+      <c r="AO121" s="12">
+        <v>17</v>
       </c>
       <c r="KB121" s="12">
-        <v>16</v>
+        <v>14</v>
       </c>
     </row>
     <row r="122" spans="1:288" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A122" s="11" t="s">
-        <v>1142</v>
+        <v>1087</v>
+      </c>
+      <c r="AO122" s="9" t="s">
+        <v>1105</v>
       </c>
       <c r="KB122" s="9" t="s">
-        <v>1173</v>
+        <v>1171</v>
       </c>
     </row>
     <row r="123" spans="1:288" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A123" s="11" t="s">
-        <v>1143</v>
+        <v>1088</v>
+      </c>
+      <c r="AO123" s="9" t="s">
+        <v>1097</v>
       </c>
       <c r="KB123" s="9" t="s">
         <v>1097</v>
@@ -15322,15 +16173,15 @@
     </row>
     <row r="124" spans="1:288" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A124" s="11" t="s">
-        <v>1156</v>
+        <v>1089</v>
       </c>
       <c r="KB124" s="9" t="s">
-        <v>1104</v>
+        <v>1103</v>
       </c>
     </row>
     <row r="125" spans="1:288" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A125" s="11" t="s">
-        <v>1157</v>
+        <v>1090</v>
       </c>
       <c r="KB125" s="9" t="s">
         <v>1167</v>
@@ -15338,23 +16189,32 @@
     </row>
     <row r="126" spans="1:288" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A126" s="10" t="s">
-        <v>1144</v>
+        <v>1091</v>
+      </c>
+      <c r="AO126" s="12">
+        <v>19</v>
       </c>
       <c r="KB126" s="12">
-        <v>17</v>
+        <v>15</v>
       </c>
     </row>
     <row r="127" spans="1:288" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A127" s="11" t="s">
-        <v>1145</v>
+        <v>1092</v>
+      </c>
+      <c r="AO127" s="9" t="s">
+        <v>1106</v>
       </c>
       <c r="KB127" s="9" t="s">
-        <v>1174</v>
+        <v>1172</v>
       </c>
     </row>
     <row r="128" spans="1:288" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A128" s="11" t="s">
-        <v>1146</v>
+        <v>1093</v>
+      </c>
+      <c r="AO128" s="9" t="s">
+        <v>1097</v>
       </c>
       <c r="KB128" s="9" t="s">
         <v>1097</v>
@@ -15362,15 +16222,15 @@
     </row>
     <row r="129" spans="1:288" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A129" s="11" t="s">
-        <v>1158</v>
+        <v>1094</v>
       </c>
       <c r="KB129" s="9" t="s">
-        <v>1104</v>
+        <v>1103</v>
       </c>
     </row>
     <row r="130" spans="1:288" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A130" s="11" t="s">
-        <v>1159</v>
+        <v>1095</v>
       </c>
       <c r="KB130" s="9" t="s">
         <v>1167</v>
@@ -15378,23 +16238,23 @@
     </row>
     <row r="131" spans="1:288" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A131" s="10" t="s">
-        <v>1147</v>
+        <v>1141</v>
       </c>
       <c r="KB131" s="12">
-        <v>18</v>
+        <v>16</v>
       </c>
     </row>
     <row r="132" spans="1:288" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A132" s="11" t="s">
-        <v>1148</v>
+        <v>1142</v>
       </c>
       <c r="KB132" s="9" t="s">
-        <v>1175</v>
+        <v>1173</v>
       </c>
     </row>
     <row r="133" spans="1:288" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A133" s="11" t="s">
-        <v>1149</v>
+        <v>1143</v>
       </c>
       <c r="KB133" s="9" t="s">
         <v>1097</v>
@@ -15402,15 +16262,15 @@
     </row>
     <row r="134" spans="1:288" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A134" s="11" t="s">
-        <v>1160</v>
+        <v>1156</v>
       </c>
       <c r="KB134" s="9" t="s">
-        <v>1105</v>
+        <v>1104</v>
       </c>
     </row>
     <row r="135" spans="1:288" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A135" s="11" t="s">
-        <v>1161</v>
+        <v>1157</v>
       </c>
       <c r="KB135" s="9" t="s">
         <v>1167</v>
@@ -15418,23 +16278,23 @@
     </row>
     <row r="136" spans="1:288" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A136" s="10" t="s">
-        <v>1150</v>
+        <v>1144</v>
       </c>
       <c r="KB136" s="12">
-        <v>19</v>
+        <v>17</v>
       </c>
     </row>
     <row r="137" spans="1:288" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A137" s="11" t="s">
-        <v>1151</v>
+        <v>1145</v>
       </c>
       <c r="KB137" s="9" t="s">
-        <v>1176</v>
+        <v>1174</v>
       </c>
     </row>
     <row r="138" spans="1:288" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A138" s="11" t="s">
-        <v>1152</v>
+        <v>1146</v>
       </c>
       <c r="KB138" s="9" t="s">
         <v>1097</v>
@@ -15442,15 +16302,15 @@
     </row>
     <row r="139" spans="1:288" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A139" s="11" t="s">
-        <v>1162</v>
+        <v>1158</v>
       </c>
       <c r="KB139" s="9" t="s">
-        <v>1105</v>
+        <v>1104</v>
       </c>
     </row>
     <row r="140" spans="1:288" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A140" s="11" t="s">
-        <v>1163</v>
+        <v>1159</v>
       </c>
       <c r="KB140" s="9" t="s">
         <v>1167</v>
@@ -15458,23 +16318,23 @@
     </row>
     <row r="141" spans="1:288" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A141" s="10" t="s">
-        <v>1153</v>
+        <v>1147</v>
       </c>
       <c r="KB141" s="12">
-        <v>20</v>
+        <v>18</v>
       </c>
     </row>
     <row r="142" spans="1:288" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A142" s="11" t="s">
-        <v>1154</v>
+        <v>1148</v>
       </c>
       <c r="KB142" s="9" t="s">
-        <v>1177</v>
+        <v>1175</v>
       </c>
     </row>
     <row r="143" spans="1:288" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A143" s="11" t="s">
-        <v>1155</v>
+        <v>1149</v>
       </c>
       <c r="KB143" s="9" t="s">
         <v>1097</v>
@@ -15482,17 +16342,97 @@
     </row>
     <row r="144" spans="1:288" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A144" s="11" t="s">
-        <v>1164</v>
+        <v>1160</v>
       </c>
       <c r="KB144" s="9" t="s">
-        <v>1106</v>
+        <v>1105</v>
       </c>
     </row>
     <row r="145" spans="1:288" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A145" s="11" t="s">
+        <v>1161</v>
+      </c>
+      <c r="KB145" s="9" t="s">
+        <v>1167</v>
+      </c>
+    </row>
+    <row r="146" spans="1:288" s="12" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A146" s="10" t="s">
+        <v>1150</v>
+      </c>
+      <c r="KB146" s="12">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="147" spans="1:288" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A147" s="11" t="s">
+        <v>1151</v>
+      </c>
+      <c r="KB147" s="9" t="s">
+        <v>1176</v>
+      </c>
+    </row>
+    <row r="148" spans="1:288" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A148" s="11" t="s">
+        <v>1152</v>
+      </c>
+      <c r="KB148" s="9" t="s">
+        <v>1097</v>
+      </c>
+    </row>
+    <row r="149" spans="1:288" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A149" s="11" t="s">
+        <v>1162</v>
+      </c>
+      <c r="KB149" s="9" t="s">
+        <v>1105</v>
+      </c>
+    </row>
+    <row r="150" spans="1:288" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A150" s="11" t="s">
+        <v>1163</v>
+      </c>
+      <c r="KB150" s="9" t="s">
+        <v>1167</v>
+      </c>
+    </row>
+    <row r="151" spans="1:288" s="12" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A151" s="10" t="s">
+        <v>1153</v>
+      </c>
+      <c r="KB151" s="12">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="152" spans="1:288" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A152" s="11" t="s">
+        <v>1154</v>
+      </c>
+      <c r="KB152" s="9" t="s">
+        <v>1177</v>
+      </c>
+    </row>
+    <row r="153" spans="1:288" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A153" s="11" t="s">
+        <v>1155</v>
+      </c>
+      <c r="KB153" s="9" t="s">
+        <v>1097</v>
+      </c>
+    </row>
+    <row r="154" spans="1:288" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A154" s="11" t="s">
+        <v>1164</v>
+      </c>
+      <c r="KB154" s="9" t="s">
+        <v>1106</v>
+      </c>
+    </row>
+    <row r="155" spans="1:288" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A155" s="11" t="s">
         <v>1165</v>
       </c>
-      <c r="KB145" s="9" t="s">
+      <c r="KB155" s="9" t="s">
         <v>1167</v>
       </c>
     </row>
@@ -15500,85 +16440,127 @@
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A62:JS70">
     <sortCondition ref="A62:A70"/>
   </sortState>
-  <conditionalFormatting sqref="LF1:LI1 A1:LD1 LP1 LS1 MA1:XFD1">
-    <cfRule type="duplicateValues" dxfId="44" priority="34"/>
+  <conditionalFormatting sqref="LF1:LI1 A1:LD1 LP1 LS1 MO1:XFD1">
+    <cfRule type="duplicateValues" dxfId="58" priority="49"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="LE1">
-    <cfRule type="duplicateValues" dxfId="43" priority="33"/>
+    <cfRule type="duplicateValues" dxfId="57" priority="48"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="LN1">
-    <cfRule type="duplicateValues" dxfId="42" priority="32"/>
+    <cfRule type="duplicateValues" dxfId="56" priority="47"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="LO1">
-    <cfRule type="duplicateValues" dxfId="41" priority="31"/>
+    <cfRule type="duplicateValues" dxfId="55" priority="46"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="A21">
-    <cfRule type="expression" dxfId="40" priority="30">
+    <cfRule type="expression" dxfId="54" priority="45">
       <formula>(COUNTA(21:21)=1)</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A71:A120">
-    <cfRule type="expression" dxfId="39" priority="53">
-      <formula>(COUNTA(71:71)=1)</formula>
+  <conditionalFormatting sqref="A81:A130">
+    <cfRule type="expression" dxfId="53" priority="68">
+      <formula>(COUNTA(81:81)=1)</formula>
     </cfRule>
-    <cfRule type="duplicateValues" dxfId="38" priority="54"/>
+    <cfRule type="duplicateValues" dxfId="52" priority="69"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A134:A135">
+    <cfRule type="expression" dxfId="51" priority="39">
+      <formula>(COUNTA(134:134)=1)</formula>
+    </cfRule>
+    <cfRule type="duplicateValues" dxfId="50" priority="40"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A139:A140">
+    <cfRule type="expression" dxfId="49" priority="37">
+      <formula>(COUNTA(139:139)=1)</formula>
+    </cfRule>
+    <cfRule type="duplicateValues" dxfId="48" priority="38"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A144:A145">
+    <cfRule type="expression" dxfId="47" priority="35">
+      <formula>(COUNTA(144:144)=1)</formula>
+    </cfRule>
+    <cfRule type="duplicateValues" dxfId="46" priority="36"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A149:A150">
+    <cfRule type="expression" dxfId="45" priority="33">
+      <formula>(COUNTA(149:149)=1)</formula>
+    </cfRule>
+    <cfRule type="duplicateValues" dxfId="44" priority="34"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A154:A155">
+    <cfRule type="expression" dxfId="43" priority="31">
+      <formula>(COUNTA(154:154)=1)</formula>
+    </cfRule>
+    <cfRule type="duplicateValues" dxfId="42" priority="32"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="LT1">
+    <cfRule type="duplicateValues" dxfId="41" priority="22"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="LU1">
+    <cfRule type="duplicateValues" dxfId="40" priority="21"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="LV1">
+    <cfRule type="duplicateValues" dxfId="39" priority="20"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="LW1">
+    <cfRule type="duplicateValues" dxfId="38" priority="19"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="LX1">
+    <cfRule type="duplicateValues" dxfId="37" priority="18"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="LY1">
+    <cfRule type="duplicateValues" dxfId="36" priority="17"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="LZ1">
+    <cfRule type="duplicateValues" dxfId="35" priority="16"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="MA1">
+    <cfRule type="duplicateValues" dxfId="34" priority="15"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="MB1">
+    <cfRule type="duplicateValues" dxfId="33" priority="14"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="MC1">
+    <cfRule type="duplicateValues" dxfId="32" priority="13"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="MD1">
+    <cfRule type="duplicateValues" dxfId="31" priority="11"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="ME1">
+    <cfRule type="duplicateValues" dxfId="30" priority="10"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="MF1">
+    <cfRule type="duplicateValues" dxfId="29" priority="9"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="MG1">
+    <cfRule type="duplicateValues" dxfId="28" priority="8"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="MH1">
+    <cfRule type="duplicateValues" dxfId="27" priority="7"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="MI1">
+    <cfRule type="duplicateValues" dxfId="26" priority="6"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="MJ1">
+    <cfRule type="duplicateValues" dxfId="25" priority="5"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="A1:A1048576">
-    <cfRule type="expression" dxfId="37" priority="26">
+    <cfRule type="expression" dxfId="24" priority="76">
       <formula>(COUNTA(1:1)=1)</formula>
     </cfRule>
-    <cfRule type="duplicateValues" dxfId="36" priority="27"/>
+    <cfRule type="duplicateValues" dxfId="23" priority="77"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A124:A125">
-    <cfRule type="expression" dxfId="35" priority="24">
-      <formula>(COUNTA(124:124)=1)</formula>
-    </cfRule>
-    <cfRule type="duplicateValues" dxfId="34" priority="25"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A129:A130">
-    <cfRule type="expression" dxfId="33" priority="22">
-      <formula>(COUNTA(129:129)=1)</formula>
-    </cfRule>
-    <cfRule type="duplicateValues" dxfId="32" priority="23"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A134:A135">
-    <cfRule type="expression" dxfId="31" priority="20">
-      <formula>(COUNTA(134:134)=1)</formula>
-    </cfRule>
-    <cfRule type="duplicateValues" dxfId="30" priority="21"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A139:A140">
-    <cfRule type="expression" dxfId="29" priority="18">
-      <formula>(COUNTA(139:139)=1)</formula>
-    </cfRule>
-    <cfRule type="duplicateValues" dxfId="28" priority="19"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A144:A145">
-    <cfRule type="expression" dxfId="27" priority="16">
-      <formula>(COUNTA(144:144)=1)</formula>
-    </cfRule>
-    <cfRule type="duplicateValues" dxfId="26" priority="17"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="LT1">
-    <cfRule type="duplicateValues" dxfId="25" priority="7"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="LU1">
-    <cfRule type="duplicateValues" dxfId="24" priority="6"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="LV1">
-    <cfRule type="duplicateValues" dxfId="23" priority="5"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="LW1">
+  <conditionalFormatting sqref="MK1">
     <cfRule type="duplicateValues" dxfId="22" priority="4"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="LX1">
+  <conditionalFormatting sqref="ML1">
     <cfRule type="duplicateValues" dxfId="21" priority="3"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="LY1">
-    <cfRule type="duplicateValues" dxfId="20" priority="2"/>
+  <conditionalFormatting sqref="MM1">
+    <cfRule type="duplicateValues" dxfId="1" priority="2"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="LZ1">
-    <cfRule type="duplicateValues" dxfId="19" priority="1"/>
+  <conditionalFormatting sqref="MN1">
+    <cfRule type="duplicateValues" dxfId="0" priority="1"/>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -70813,63 +71795,63 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="A318:A321 A1:A316 A328 A331">
-    <cfRule type="duplicateValues" dxfId="18" priority="17"/>
+    <cfRule type="duplicateValues" dxfId="20" priority="17"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="A317">
-    <cfRule type="duplicateValues" dxfId="17" priority="16"/>
+    <cfRule type="duplicateValues" dxfId="19" priority="16"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="A326">
-    <cfRule type="duplicateValues" dxfId="16" priority="15"/>
+    <cfRule type="duplicateValues" dxfId="18" priority="15"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="A327">
-    <cfRule type="duplicateValues" dxfId="15" priority="14"/>
+    <cfRule type="duplicateValues" dxfId="17" priority="14"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="U1">
-    <cfRule type="expression" dxfId="14" priority="13">
+    <cfRule type="expression" dxfId="16" priority="13">
       <formula>(COUNTA(1:1)=1)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="BS1:DP1">
-    <cfRule type="expression" dxfId="13" priority="18">
+    <cfRule type="expression" dxfId="15" priority="18">
       <formula>(COUNTA(1:1)=1)</formula>
     </cfRule>
-    <cfRule type="duplicateValues" dxfId="12" priority="19"/>
+    <cfRule type="duplicateValues" dxfId="14" priority="19"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="A1:EO1">
-    <cfRule type="expression" dxfId="11" priority="11">
+    <cfRule type="expression" dxfId="13" priority="11">
       <formula>(COUNTA(1:1)=1)</formula>
     </cfRule>
-    <cfRule type="duplicateValues" dxfId="10" priority="12"/>
+    <cfRule type="duplicateValues" dxfId="12" priority="12"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="DT1:DU1">
-    <cfRule type="expression" dxfId="9" priority="9">
+    <cfRule type="expression" dxfId="11" priority="9">
       <formula>(COUNTA(1:1)=1)</formula>
     </cfRule>
-    <cfRule type="duplicateValues" dxfId="8" priority="10"/>
+    <cfRule type="duplicateValues" dxfId="10" priority="10"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="DY1:DZ1">
-    <cfRule type="expression" dxfId="7" priority="7">
+    <cfRule type="expression" dxfId="9" priority="7">
       <formula>(COUNTA(1:1)=1)</formula>
     </cfRule>
-    <cfRule type="duplicateValues" dxfId="6" priority="8"/>
+    <cfRule type="duplicateValues" dxfId="8" priority="8"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="ED1:EE1">
-    <cfRule type="expression" dxfId="5" priority="5">
+    <cfRule type="expression" dxfId="7" priority="5">
       <formula>(COUNTA(1:1)=1)</formula>
     </cfRule>
-    <cfRule type="duplicateValues" dxfId="4" priority="6"/>
+    <cfRule type="duplicateValues" dxfId="6" priority="6"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="EI1:EJ1">
-    <cfRule type="expression" dxfId="3" priority="3">
+    <cfRule type="expression" dxfId="5" priority="3">
       <formula>(COUNTA(1:1)=1)</formula>
     </cfRule>
-    <cfRule type="duplicateValues" dxfId="2" priority="4"/>
+    <cfRule type="duplicateValues" dxfId="4" priority="4"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="EN1:EO1">
-    <cfRule type="expression" dxfId="1" priority="1">
+    <cfRule type="expression" dxfId="3" priority="1">
       <formula>(COUNTA(1:1)=1)</formula>
     </cfRule>
-    <cfRule type="duplicateValues" dxfId="0" priority="2"/>
+    <cfRule type="duplicateValues" dxfId="2" priority="2"/>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Various changes Started experimenting with cached calculations
</commit_message>
<xml_diff>
--- a/activities.xlsx
+++ b/activities.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24527"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24701"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/eb76e5660c890129/Personal/Projects/Design/PECS/work assets/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="2184" documentId="13_ncr:40009_{E3EB266C-7612-416D-8781-7A2BED99FA57}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{06C059BE-9BEC-42FE-8779-7DC9B3F65BF0}"/>
+  <xr:revisionPtr revIDLastSave="2186" documentId="13_ncr:40009_{E3EB266C-7612-416D-8781-7A2BED99FA57}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{1703CB57-A930-4F96-B7EE-0B346AE7B212}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="57840" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2295" yWindow="2295" windowWidth="43200" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Work" sheetId="2" r:id="rId1"/>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6527" uniqueCount="1327">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6527" uniqueCount="1328">
   <si>
     <t>name</t>
   </si>
@@ -4145,6 +4145,13 @@
   </si>
   <si>
     <t>gainConditions/0/increaseRadius</t>
+  </si>
+  <si>
+    <t>You tap into your inner fury and begin raging. You gain a number of temporary Hit Points equal to your level plus your Constitution modifier. This frenzy lasts for 1 minute, until there are no enemies you can perceive, or until you fall unconscious, whichever comes first. You can't voluntarily stop raging. While you are raging:
+You deal 2 additional damage with melee weapons and unarmed attacks. This additional damage is halved if your weapon or unarmed attack is agile.
+You take a -1 penalty to AC.
+You can't use actions with the concentrate trait unless they also have the rage trait. You can Seek while raging.
+After you stop raging, you lose any remaining temporary Hit Points from Rage, and you can't Rage again for 1 minute.</t>
   </si>
 </sst>
 </file>
@@ -5401,10 +5408,10 @@
   <dimension ref="A1:MT154"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="MK2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="BJ25" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="MT3" sqref="MT3"/>
+      <selection pane="bottomRight" activeCell="BO25" sqref="BO25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -12731,7 +12738,7 @@
         <v>284</v>
       </c>
       <c r="BO25" s="1" t="s">
-        <v>288</v>
+        <v>1327</v>
       </c>
       <c r="BP25" s="1" t="s">
         <v>291</v>

</xml_diff>

<commit_message>
A lot of content
</commit_message>
<xml_diff>
--- a/activities.xlsx
+++ b/activities.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24701"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24827"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/eb76e5660c890129/Personal/Projects/Design/PECS/work assets/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="2186" documentId="13_ncr:40009_{E3EB266C-7612-416D-8781-7A2BED99FA57}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{1703CB57-A930-4F96-B7EE-0B346AE7B212}"/>
+  <xr:revisionPtr revIDLastSave="2198" documentId="13_ncr:40009_{E3EB266C-7612-416D-8781-7A2BED99FA57}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{89BEE23D-1C36-437E-82BE-1DCD5C989EDE}"/>
   <bookViews>
-    <workbookView xWindow="2295" yWindow="2295" windowWidth="43200" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1635" yWindow="1245" windowWidth="57600" windowHeight="15345" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Work" sheetId="2" r:id="rId1"/>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6527" uniqueCount="1328">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6532" uniqueCount="1331">
   <si>
     <t>name</t>
   </si>
@@ -4152,6 +4152,16 @@
 You take a -1 penalty to AC.
 You can't use actions with the concentrate trait unless they also have the rage trait. You can Seek while raging.
 After you stop raging, you lose any remaining temporary Hit Points from Rage, and you can't Rage again for 1 minute.</t>
+  </si>
+  <si>
+    <t>Sun Wheel: Fire Damage</t>
+  </si>
+  <si>
+    <t>When you use the shield spell granted by the sun wheel to prevent damage, if the attacker is adjacent to you, you can choose to deal |dice=2d6 Fire| 2d6 fire damage to it, which it gets a DC 21 basic Reflex save to resist.
+If you choose to deal the fire damage, you can't Activate the sun wheel again until the next morning.</t>
+  </si>
+  <si>
+    <t>Sun Wheel Cooldown</t>
   </si>
 </sst>
 </file>
@@ -5405,23 +5415,23 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:MT154"/>
+  <dimension ref="A1:MU154"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="BJ25" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="MM17" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="BO25" sqref="BO25"/>
+      <selection pane="bottomRight" activeCell="MU42" sqref="MU42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="37.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="358" width="27.42578125" style="1" customWidth="1"/>
-    <col min="359" max="16384" width="9.140625" style="1"/>
+    <col min="2" max="359" width="27.42578125" style="1" customWidth="1"/>
+    <col min="360" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:358" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:359" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -6496,8 +6506,11 @@
       <c r="MT1" t="s">
         <v>1323</v>
       </c>
+      <c r="MU1" t="s">
+        <v>1328</v>
+      </c>
     </row>
-    <row r="2" spans="1:358" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:359" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>1</v>
       </c>
@@ -7543,7 +7556,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="3" spans="1:358" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:359" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>20</v>
       </c>
@@ -7770,7 +7783,7 @@
         <v>1321</v>
       </c>
     </row>
-    <row r="4" spans="1:358" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:359" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
         <v>3</v>
       </c>
@@ -8780,7 +8793,7 @@
         <v>1318</v>
       </c>
     </row>
-    <row r="5" spans="1:358" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:359" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
         <v>4</v>
       </c>
@@ -9481,7 +9494,7 @@
         <v>142</v>
       </c>
     </row>
-    <row r="6" spans="1:358" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:359" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
         <v>11</v>
       </c>
@@ -9849,7 +9862,7 @@
         <v>314</v>
       </c>
     </row>
-    <row r="7" spans="1:358" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:359" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
         <v>12</v>
       </c>
@@ -10088,7 +10101,7 @@
         <v>314</v>
       </c>
     </row>
-    <row r="8" spans="1:358" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:359" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
         <v>13</v>
       </c>
@@ -10234,7 +10247,7 @@
         <v>179</v>
       </c>
     </row>
-    <row r="9" spans="1:358" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:359" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
         <v>34</v>
       </c>
@@ -10260,7 +10273,7 @@
         <v>287</v>
       </c>
     </row>
-    <row r="10" spans="1:358" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:359" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
         <v>37</v>
       </c>
@@ -10274,7 +10287,7 @@
         <v>894</v>
       </c>
     </row>
-    <row r="11" spans="1:358" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:359" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
         <v>6</v>
       </c>
@@ -10579,7 +10592,7 @@
         <v>1266</v>
       </c>
     </row>
-    <row r="12" spans="1:358" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:359" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
         <v>10</v>
       </c>
@@ -10812,7 +10825,7 @@
         <v>1267</v>
       </c>
     </row>
-    <row r="13" spans="1:358" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:359" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
         <v>5</v>
       </c>
@@ -10967,12 +10980,12 @@
         <v>1</v>
       </c>
     </row>
-    <row r="14" spans="1:358" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:359" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
         <v>934</v>
       </c>
     </row>
-    <row r="15" spans="1:358" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:359" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
         <v>46</v>
       </c>
@@ -10986,7 +10999,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="16" spans="1:358" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:359" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
         <v>35</v>
       </c>
@@ -10997,7 +11010,7 @@
         <v>1202</v>
       </c>
     </row>
-    <row r="17" spans="1:358" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:359" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
         <v>18</v>
       </c>
@@ -11120,7 +11133,7 @@
         <v>1278</v>
       </c>
     </row>
-    <row r="18" spans="1:358" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:359" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
         <v>19</v>
       </c>
@@ -11254,7 +11267,7 @@
         <v>1000</v>
       </c>
     </row>
-    <row r="19" spans="1:358" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:359" x14ac:dyDescent="0.25">
       <c r="A19" s="1" t="s">
         <v>36</v>
       </c>
@@ -11265,7 +11278,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="20" spans="1:358" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:359" x14ac:dyDescent="0.25">
       <c r="A20" s="1" t="s">
         <v>21</v>
       </c>
@@ -11315,7 +11328,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="21" spans="1:358" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:359" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>1014</v>
       </c>
@@ -11335,7 +11348,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="22" spans="1:358" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:359" x14ac:dyDescent="0.25">
       <c r="A22" s="1" t="s">
         <v>1012</v>
       </c>
@@ -12410,8 +12423,11 @@
       <c r="MT22" s="1" t="s">
         <v>995</v>
       </c>
+      <c r="MU22" s="1" t="s">
+        <v>994</v>
+      </c>
     </row>
-    <row r="23" spans="1:358" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:359" x14ac:dyDescent="0.25">
       <c r="A23" s="1" t="s">
         <v>1028</v>
       </c>
@@ -12443,7 +12459,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="24" spans="1:358" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:359" x14ac:dyDescent="0.25">
       <c r="A24" s="1" t="s">
         <v>1184</v>
       </c>
@@ -12538,7 +12554,7 @@
         <v>1225</v>
       </c>
     </row>
-    <row r="25" spans="1:358" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:359" x14ac:dyDescent="0.25">
       <c r="A25" s="1" t="s">
         <v>2</v>
       </c>
@@ -13613,8 +13629,11 @@
       <c r="MT25" t="s">
         <v>1322</v>
       </c>
+      <c r="MU25" s="1" t="s">
+        <v>1329</v>
+      </c>
     </row>
-    <row r="26" spans="1:358" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:359" x14ac:dyDescent="0.25">
       <c r="A26" s="1" t="s">
         <v>38</v>
       </c>
@@ -13631,7 +13650,7 @@
         <v>698</v>
       </c>
     </row>
-    <row r="27" spans="1:358" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:359" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A27" s="3" t="s">
         <v>14</v>
       </c>
@@ -13684,7 +13703,7 @@
         <v>1250</v>
       </c>
     </row>
-    <row r="28" spans="1:358" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:359" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A28" s="3" t="s">
         <v>15</v>
       </c>
@@ -13746,7 +13765,7 @@
         <v>1251</v>
       </c>
     </row>
-    <row r="29" spans="1:358" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:359" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A29" s="3" t="s">
         <v>16</v>
       </c>
@@ -13814,7 +13833,7 @@
         <v>1252</v>
       </c>
     </row>
-    <row r="30" spans="1:358" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:359" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A30" s="3" t="s">
         <v>17</v>
       </c>
@@ -13867,7 +13886,7 @@
         <v>1253</v>
       </c>
     </row>
-    <row r="31" spans="1:358" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:359" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A31" s="9" t="s">
         <v>1002</v>
       </c>
@@ -13887,7 +13906,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="32" spans="1:358" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:359" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A32" s="9" t="s">
         <v>1293</v>
       </c>
@@ -13895,7 +13914,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="33" spans="1:358" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:359" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A33" s="9" t="s">
         <v>1294</v>
       </c>
@@ -13903,7 +13922,7 @@
         <v>1295</v>
       </c>
     </row>
-    <row r="34" spans="1:358" s="7" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:359" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A34" s="7" t="s">
         <v>25</v>
       </c>
@@ -13914,7 +13933,7 @@
         <v>230</v>
       </c>
     </row>
-    <row r="35" spans="1:358" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:359" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A35" s="4" t="s">
         <v>22</v>
       </c>
@@ -13928,7 +13947,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="36" spans="1:358" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:359" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A36" s="4" t="s">
         <v>1326</v>
       </c>
@@ -13936,12 +13955,12 @@
         <v>10</v>
       </c>
     </row>
-    <row r="37" spans="1:358" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:359" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A37" s="4" t="s">
         <v>923</v>
       </c>
     </row>
-    <row r="38" spans="1:358" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:359" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A38" s="4" t="s">
         <v>993</v>
       </c>
@@ -13949,12 +13968,12 @@
         <v>991</v>
       </c>
     </row>
-    <row r="39" spans="1:358" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:359" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A39" s="4" t="s">
         <v>935</v>
       </c>
     </row>
-    <row r="40" spans="1:358" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:359" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A40" s="4" t="s">
         <v>7</v>
       </c>
@@ -14330,8 +14349,11 @@
       <c r="MT40" s="4">
         <v>0</v>
       </c>
+      <c r="MU40" s="4">
+        <v>-2</v>
+      </c>
     </row>
-    <row r="41" spans="1:358" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:359" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A41" s="4" t="s">
         <v>992</v>
       </c>
@@ -14339,7 +14361,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="42" spans="1:358" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:359" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A42" s="4" t="s">
         <v>8</v>
       </c>
@@ -14739,8 +14761,11 @@
       <c r="MT42" s="4" t="s">
         <v>1325</v>
       </c>
+      <c r="MU42" s="4" t="s">
+        <v>1330</v>
+      </c>
     </row>
-    <row r="43" spans="1:358" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:359" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A43" s="4" t="s">
         <v>1010</v>
       </c>
@@ -14837,8 +14862,11 @@
       <c r="MH43" s="4" t="s">
         <v>1011</v>
       </c>
+      <c r="MU43" s="4" t="s">
+        <v>1011</v>
+      </c>
     </row>
-    <row r="44" spans="1:358" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:359" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A44" s="4" t="s">
         <v>989</v>
       </c>
@@ -14846,7 +14874,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="45" spans="1:358" s="7" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:359" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A45" s="7" t="s">
         <v>29</v>
       </c>
@@ -14854,17 +14882,17 @@
         <v>189</v>
       </c>
     </row>
-    <row r="46" spans="1:358" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:359" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A46" s="4" t="s">
         <v>924</v>
       </c>
     </row>
-    <row r="47" spans="1:358" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:359" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A47" s="4" t="s">
         <v>937</v>
       </c>
     </row>
-    <row r="48" spans="1:358" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:359" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A48" s="4" t="s">
         <v>1017</v>
       </c>
@@ -15201,7 +15229,7 @@
         <v>950</v>
       </c>
     </row>
-    <row r="65" spans="1:358" s="8" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:359" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A65" s="8" t="s">
         <v>42</v>
       </c>
@@ -15209,7 +15237,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="66" spans="1:358" s="6" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:359" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A66" s="6" t="s">
         <v>41</v>
       </c>
@@ -15217,7 +15245,7 @@
         <v>628</v>
       </c>
     </row>
-    <row r="67" spans="1:358" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:359" x14ac:dyDescent="0.25">
       <c r="A67" s="1" t="s">
         <v>47</v>
       </c>
@@ -15225,7 +15253,7 @@
         <v>813</v>
       </c>
     </row>
-    <row r="68" spans="1:358" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:359" x14ac:dyDescent="0.25">
       <c r="A68" s="1" t="s">
         <v>44</v>
       </c>
@@ -15251,7 +15279,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="69" spans="1:358" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:359" x14ac:dyDescent="0.25">
       <c r="A69" s="1" t="s">
         <v>43</v>
       </c>
@@ -15277,7 +15305,7 @@
         <v>1261</v>
       </c>
     </row>
-    <row r="70" spans="1:358" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:359" x14ac:dyDescent="0.25">
       <c r="A70" s="1" t="s">
         <v>1255</v>
       </c>
@@ -15285,7 +15313,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="71" spans="1:358" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:359" x14ac:dyDescent="0.25">
       <c r="A71" s="1" t="s">
         <v>1256</v>
       </c>
@@ -15293,7 +15321,7 @@
         <v>1254</v>
       </c>
     </row>
-    <row r="72" spans="1:358" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:359" x14ac:dyDescent="0.25">
       <c r="A72" s="1" t="s">
         <v>1257</v>
       </c>
@@ -15301,7 +15329,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="73" spans="1:358" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:359" x14ac:dyDescent="0.25">
       <c r="A73" s="1" t="s">
         <v>1258</v>
       </c>
@@ -15309,7 +15337,7 @@
         <v>1261</v>
       </c>
     </row>
-    <row r="74" spans="1:358" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:359" x14ac:dyDescent="0.25">
       <c r="A74" s="1" t="s">
         <v>1259</v>
       </c>
@@ -15317,7 +15345,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="75" spans="1:358" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:359" x14ac:dyDescent="0.25">
       <c r="A75" s="1" t="s">
         <v>1260</v>
       </c>
@@ -15325,7 +15353,7 @@
         <v>1254</v>
       </c>
     </row>
-    <row r="76" spans="1:358" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:359" x14ac:dyDescent="0.25">
       <c r="A76" s="1" t="s">
         <v>1262</v>
       </c>
@@ -15333,7 +15361,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="77" spans="1:358" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:359" x14ac:dyDescent="0.25">
       <c r="A77" s="1" t="s">
         <v>1263</v>
       </c>
@@ -15341,7 +15369,7 @@
         <v>1261</v>
       </c>
     </row>
-    <row r="78" spans="1:358" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:359" x14ac:dyDescent="0.25">
       <c r="A78" s="1" t="s">
         <v>1264</v>
       </c>
@@ -15349,7 +15377,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="79" spans="1:358" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:359" x14ac:dyDescent="0.25">
       <c r="A79" s="1" t="s">
         <v>1265</v>
       </c>
@@ -15357,7 +15385,7 @@
         <v>1254</v>
       </c>
     </row>
-    <row r="80" spans="1:358" s="12" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:359" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A80" s="10" t="s">
         <v>1041</v>
       </c>
@@ -15381,8 +15409,9 @@
       <c r="MT80" s="10">
         <v>4</v>
       </c>
+      <c r="MU80" s="10"/>
     </row>
-    <row r="81" spans="1:358" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:359" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A81" s="11" t="s">
         <v>1042</v>
       </c>
@@ -15406,8 +15435,9 @@
       <c r="MT81" s="11">
         <v>4</v>
       </c>
+      <c r="MU81" s="11"/>
     </row>
-    <row r="82" spans="1:358" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:359" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A82" s="11" t="s">
         <v>1043</v>
       </c>
@@ -15431,8 +15461,9 @@
       <c r="MT82" s="11" t="s">
         <v>1092</v>
       </c>
+      <c r="MU82" s="11"/>
     </row>
-    <row r="83" spans="1:358" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:359" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A83" s="11" t="s">
         <v>1044</v>
       </c>
@@ -15446,8 +15477,9 @@
       <c r="MR83" s="11"/>
       <c r="MS83" s="11"/>
       <c r="MT83" s="11"/>
+      <c r="MU83" s="11"/>
     </row>
-    <row r="84" spans="1:358" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:359" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A84" s="11" t="s">
         <v>1045</v>
       </c>
@@ -15463,8 +15495,9 @@
       <c r="MR84" s="11"/>
       <c r="MS84" s="11"/>
       <c r="MT84" s="11"/>
+      <c r="MU84" s="11"/>
     </row>
-    <row r="85" spans="1:358" s="12" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:359" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A85" s="10" t="s">
         <v>1046</v>
       </c>
@@ -15488,8 +15521,9 @@
       <c r="MT85" s="10">
         <v>5</v>
       </c>
+      <c r="MU85" s="10"/>
     </row>
-    <row r="86" spans="1:358" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:359" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A86" s="11" t="s">
         <v>1047</v>
       </c>
@@ -15513,8 +15547,9 @@
       <c r="MT86" s="11">
         <v>5</v>
       </c>
+      <c r="MU86" s="11"/>
     </row>
-    <row r="87" spans="1:358" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:359" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A87" s="11" t="s">
         <v>1048</v>
       </c>
@@ -15538,8 +15573,9 @@
       <c r="MT87" s="11" t="s">
         <v>1092</v>
       </c>
+      <c r="MU87" s="11"/>
     </row>
-    <row r="88" spans="1:358" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:359" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A88" s="11" t="s">
         <v>1049</v>
       </c>
@@ -15555,8 +15591,9 @@
       <c r="MR88" s="11"/>
       <c r="MS88" s="11"/>
       <c r="MT88" s="11"/>
+      <c r="MU88" s="11"/>
     </row>
-    <row r="89" spans="1:358" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:359" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A89" s="11" t="s">
         <v>1050</v>
       </c>
@@ -15572,8 +15609,9 @@
       <c r="MR89" s="11"/>
       <c r="MS89" s="11"/>
       <c r="MT89" s="11"/>
+      <c r="MU89" s="11"/>
     </row>
-    <row r="90" spans="1:358" s="12" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:359" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A90" s="10" t="s">
         <v>1051</v>
       </c>
@@ -15597,8 +15635,9 @@
       <c r="MT90" s="10">
         <v>6</v>
       </c>
+      <c r="MU90" s="10"/>
     </row>
-    <row r="91" spans="1:358" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:359" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A91" s="11" t="s">
         <v>1052</v>
       </c>
@@ -15622,8 +15661,9 @@
       <c r="MT91" s="11">
         <v>6</v>
       </c>
+      <c r="MU91" s="11"/>
     </row>
-    <row r="92" spans="1:358" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:359" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A92" s="11" t="s">
         <v>1053</v>
       </c>
@@ -15647,8 +15687,9 @@
       <c r="MT92" s="11" t="s">
         <v>1092</v>
       </c>
+      <c r="MU92" s="11"/>
     </row>
-    <row r="93" spans="1:358" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:359" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A93" s="11" t="s">
         <v>1054</v>
       </c>
@@ -15664,8 +15705,9 @@
       <c r="MR93" s="11"/>
       <c r="MS93" s="11"/>
       <c r="MT93" s="11"/>
+      <c r="MU93" s="11"/>
     </row>
-    <row r="94" spans="1:358" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:359" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A94" s="11" t="s">
         <v>1055</v>
       </c>
@@ -15681,8 +15723,9 @@
       <c r="MR94" s="11"/>
       <c r="MS94" s="11"/>
       <c r="MT94" s="11"/>
+      <c r="MU94" s="11"/>
     </row>
-    <row r="95" spans="1:358" s="12" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:359" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A95" s="10" t="s">
         <v>1056</v>
       </c>
@@ -15702,7 +15745,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="96" spans="1:358" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:359" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A96" s="11" t="s">
         <v>1057</v>
       </c>
@@ -16433,7 +16476,7 @@
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A63:JS69">
     <sortCondition ref="A63:A69"/>
   </sortState>
-  <conditionalFormatting sqref="A1:MN1 MQ1 MU1:XFD1">
+  <conditionalFormatting sqref="MV1:XFD1 A1:MN1 MQ1">
     <cfRule type="duplicateValues" dxfId="45" priority="57"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="A21">
@@ -16501,7 +16544,7 @@
   <conditionalFormatting sqref="MS1">
     <cfRule type="duplicateValues" dxfId="24" priority="2"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="MT1">
+  <conditionalFormatting sqref="MT1:MU1">
     <cfRule type="duplicateValues" dxfId="23" priority="1"/>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Created csv-to-json conversion script Worn items
</commit_message>
<xml_diff>
--- a/activities.xlsx
+++ b/activities.xlsx
@@ -10,7 +10,7 @@
   </mc:AlternateContent>
   <xr:revisionPtr revIDLastSave="2199" documentId="13_ncr:40009_{E3EB266C-7612-416D-8781-7A2BED99FA57}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{FD98EE0A-4250-47B7-8D61-08BFA29FDC52}"/>
   <bookViews>
-    <workbookView xWindow="705" yWindow="2295" windowWidth="15000" windowHeight="8850" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="690" yWindow="4935" windowWidth="15015" windowHeight="6210" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Work" sheetId="2" r:id="rId1"/>
@@ -5421,10 +5421,10 @@
   <dimension ref="A1:MU154"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="AU14" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="DP28" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="AZ34" sqref="AZ34"/>
+      <selection pane="bottomRight" activeCell="DS49" sqref="DS49"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
csv-to-json script now adds _extensionFileName
</commit_message>
<xml_diff>
--- a/activities.xlsx
+++ b/activities.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\OneDrive\Personal\Projects\Design\PECS\work assets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{96A65CF8-03D3-4266-9083-11FAB3DB817C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C75AE77F-DDAF-4A39-906D-E528291017AD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3135" yWindow="3210" windowWidth="33420" windowHeight="16485" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="3825" yWindow="3900" windowWidth="33420" windowHeight="16485" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Work" sheetId="2" r:id="rId1"/>
@@ -4672,7 +4672,207 @@
     <cellStyle name="Total" xfId="17" builtinId="25" customBuiltin="1"/>
     <cellStyle name="Warning Text" xfId="14" builtinId="11" customBuiltin="1"/>
   </cellStyles>
-  <dxfs count="46">
+  <dxfs count="69">
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="6" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <font>
         <color rgb="FF9C0006"/>
@@ -5385,11 +5585,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:MU154"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="MO73" activePane="bottomRight" state="frozen"/>
+    <sheetView workbookViewId="0">
+      <pane xSplit="1" ySplit="1" topLeftCell="MM116" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="MQ85" sqref="MQ85"/>
+      <selection pane="bottomRight" sqref="A1:MU154"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -16439,75 +16639,75 @@
     <sortCondition ref="A63:A69"/>
   </sortState>
   <conditionalFormatting sqref="MV1:XFD1 A1:MN1 MQ1">
-    <cfRule type="duplicateValues" dxfId="45" priority="57"/>
+    <cfRule type="duplicateValues" dxfId="68" priority="57"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="A21">
-    <cfRule type="expression" dxfId="44" priority="53">
+    <cfRule type="expression" dxfId="67" priority="53">
       <formula>(COUNTA(21:21)=1)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A80:A129">
-    <cfRule type="expression" dxfId="43" priority="76">
+    <cfRule type="expression" dxfId="66" priority="76">
       <formula>(COUNTA(80:80)=1)</formula>
     </cfRule>
-    <cfRule type="duplicateValues" dxfId="42" priority="77"/>
+    <cfRule type="duplicateValues" dxfId="65" priority="77"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="A133:A134">
-    <cfRule type="expression" dxfId="41" priority="47">
+    <cfRule type="expression" dxfId="64" priority="47">
       <formula>(COUNTA(133:133)=1)</formula>
     </cfRule>
-    <cfRule type="duplicateValues" dxfId="40" priority="48"/>
+    <cfRule type="duplicateValues" dxfId="63" priority="48"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="A138:A139">
-    <cfRule type="expression" dxfId="39" priority="45">
+    <cfRule type="expression" dxfId="62" priority="45">
       <formula>(COUNTA(138:138)=1)</formula>
     </cfRule>
-    <cfRule type="duplicateValues" dxfId="38" priority="46"/>
+    <cfRule type="duplicateValues" dxfId="61" priority="46"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="A143:A144">
-    <cfRule type="expression" dxfId="37" priority="43">
+    <cfRule type="expression" dxfId="60" priority="43">
       <formula>(COUNTA(143:143)=1)</formula>
     </cfRule>
-    <cfRule type="duplicateValues" dxfId="36" priority="44"/>
+    <cfRule type="duplicateValues" dxfId="59" priority="44"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="A148:A149">
-    <cfRule type="expression" dxfId="35" priority="41">
+    <cfRule type="expression" dxfId="58" priority="41">
       <formula>(COUNTA(148:148)=1)</formula>
     </cfRule>
-    <cfRule type="duplicateValues" dxfId="34" priority="42"/>
+    <cfRule type="duplicateValues" dxfId="57" priority="42"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="A153:A154">
-    <cfRule type="expression" dxfId="33" priority="39">
+    <cfRule type="expression" dxfId="56" priority="39">
       <formula>(COUNTA(153:153)=1)</formula>
     </cfRule>
-    <cfRule type="duplicateValues" dxfId="32" priority="40"/>
+    <cfRule type="duplicateValues" dxfId="55" priority="40"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="MO1">
-    <cfRule type="duplicateValues" dxfId="31" priority="5"/>
-    <cfRule type="expression" dxfId="30" priority="6">
+    <cfRule type="duplicateValues" dxfId="54" priority="5"/>
+    <cfRule type="expression" dxfId="53" priority="6">
       <formula>NOT(ISERROR(FIND("(Caster)",MO1)))</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="29" priority="7">
+    <cfRule type="expression" dxfId="52" priority="7">
       <formula>ISBLANK(MO2)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="MP1">
-    <cfRule type="duplicateValues" dxfId="28" priority="4"/>
+    <cfRule type="duplicateValues" dxfId="51" priority="4"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="A1:A1048576">
-    <cfRule type="expression" dxfId="27" priority="90">
+    <cfRule type="expression" dxfId="50" priority="90">
       <formula>(COUNTA(1:1)=1)</formula>
     </cfRule>
-    <cfRule type="duplicateValues" dxfId="26" priority="91"/>
+    <cfRule type="duplicateValues" dxfId="49" priority="91"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="MR1">
-    <cfRule type="duplicateValues" dxfId="25" priority="3"/>
+    <cfRule type="duplicateValues" dxfId="48" priority="3"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="MS1">
-    <cfRule type="duplicateValues" dxfId="24" priority="2"/>
+    <cfRule type="duplicateValues" dxfId="47" priority="2"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="MT1:MU1">
-    <cfRule type="duplicateValues" dxfId="23" priority="1"/>
+    <cfRule type="duplicateValues" dxfId="46" priority="1"/>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -16518,7 +16718,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:EX359"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection sqref="A1:EX359"/>
     </sheetView>
   </sheetViews>
@@ -69391,7 +69591,7 @@
         <v>7</v>
       </c>
       <c r="CH355" s="11">
-        <v>20</v>
+        <v>15</v>
       </c>
       <c r="CI355" s="11" t="s">
         <v>1083</v>
@@ -69403,7 +69603,7 @@
         <v>1133</v>
       </c>
       <c r="CL355" s="10">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="CM355" s="11">
         <v>20</v>

</xml_diff>